<commit_message>
Updating rGC homology analysis
</commit_message>
<xml_diff>
--- a/Code/rGC Homology/Ce-rGC_tBlastn.xlsx
+++ b/Code/rGC Homology/Ce-rGC_tBlastn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astrasb/Documents/RStudio/Bryant_et_al_2021/Code/rGC Homology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B68C7C9-43CE-484D-8A85-692BD6751448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9B0C10-E67D-0F44-ADBF-9C85621B2B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="12040" windowWidth="34900" windowHeight="8180" activeTab="5" xr2:uid="{AD4C77C0-16BB-4E4E-91C7-9E778F091754}"/>
+    <workbookView xWindow="180" yWindow="1520" windowWidth="34900" windowHeight="11100" activeTab="5" xr2:uid="{AD4C77C0-16BB-4E4E-91C7-9E778F091754}"/>
   </bookViews>
   <sheets>
     <sheet name="Ce_to_Sr" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="248">
   <si>
     <t>DAF-11</t>
   </si>
@@ -555,9 +555,6 @@
     <t>MVSIIILLIILTTKVFPKSVGILKVGLIFPNIEPVLIKYMGYQNSASAVVIAFKEAKKEYPILKNLTIEIVCDYTECLSFEVSGKAYDLIKKNKINVLIGPPCKKTMEIVSSIATYYNIVTLFWGNTFTYLPNKYNDKNIVGNIMGTYSDMNHCLANILLKFDWVSISLIYQSTYYELEMCEKYSESFQNILTTYYEDILIVYRKKIVSTKKEDLKEIADDIKKVSRIIIMCFSEREKEEKMLLQFYDNNMNNQDYVYINIDCSMVAYEDSKNQKLINTLDVHLNNNDKKLLSMYKWIYNFKFSLNGMRGHLYSDVKKSVPKLMKESPFYCIEECSEYNTSSHYAPYLFDAAYIYFLTIGNLLSSQKVANFSNISYKNIIKKIPGHYNGATGLYRINKNLTRDTEVTFSRYDYYNNSIIHLIKGSRTENATIITYLYTDPKTTIWYYRNGEQPLNVPKCGYSEELCQPTFIESSPIGFAGIILGSIIIILIIIGSIIYGFYTKFKQEKLDNLIWKIDTLDITNYSNYIAKKNEGQSKISLLSSICSNGKTNFQSLEERKHILYIYKRKIIVGTKHEVHYTLNKKDTIELRNLKMLNDNHLNQFIGFYNSPSYSISFWRYCPRLSLVDVFQLESLKSKIDNFFIYSFISDAIDGMEIIHKSPIKVHGNLMLNNCLVDERWKLKLSDFGMRFIREREKRDKKDLLWTAPELLKEEILQPNQNSDIYSLAIVMVDIINNNISYCNSKNEIEIDEVIYMLKNKKNEFFRPEISPVVDNIPNTMFHLIEEMWAQDPNTRPSIGVVNKLIKSMNPSKSNNLMDHIFNILEDNAITLEEEINLRTNELIKEKTKADLLLSRMLPKQVVEKLKSGQLIQPEYFDSVTVFFSDIVSFTVIASKCTPLQTVDLLNNLYTLFDSTISKHDVYKVETIGDGYMCVSGLPIKNGDLHVKEIACLSIDLVKKMPEFDVSYLPKGTVKVRIGIHSGSCIAGVVGLTMPKYCLFGDTVNIGSKIESTGKANQIHMSDKAHLLLTQKIGGFVTESQGEIIVKGAGVMNTYWLLGTEDEIIYTPIK*</t>
   </si>
   <si>
-    <t>MLYYFKYIIILYLSIFAHSKTDISLGFLFPRNSTLLESTSGFVRSAGVVTLVFEKIKKESILPDYNYDFNVFYDECDEYRATSGTYELIKYHNVDVIFGSTCNAASIRSTLMAKFYNKPTFVWGAVSSSDIAHRNRLPNIFSIFPIFLSLAYATIDVLEQFNWTTISVIYNSNPVKRCKNLFTDFEHTLTLTNTKVRIVYSLQTSFEPTPNEFDDYFFEVKDKARIIVSCFDNFKYKRKFLISMYENGLNNNEWVHINMDYRNLGFFTNIEDSLGNYSPFYKDVYDNPPDGKDDIAFEMAKKMLSVDMSTKLALSSIDDSEILENVKKWPFYCEDCNISSNTTLSTYAWYLYDAIYFWAFLINKTLPLYGDKIFNNYTLLYNHCPGNYNGMTGEINFGNTCVRAPFIILRGLDDNEETPGYITYNFSSISDYFKNVVVENFQEIMFKNWDNQIPLNVPICGYRGNLCPIDIFKDYLTEVIIVAVIITLLFLFIVFLIIFLLWRTNRKKEEEMSRWIIPYISLTKPVPEKKEYEKSLNSLASNTYSFSSKKTFNNMNETNKYIFAYLNGEGVAGEKHKNLFQTSKNDKIELSKLIKWEHDNVNKFYGMCLDYMHPISLWKYCSRGSILIYYKLTILFLMDSF*</t>
-  </si>
-  <si>
     <t>ELETLYTNEKDTIWATRNGIKPLSVPLCGFLNENCQKSFIENYPILFGAIIFVSILIIILIILIISYMHYLKIKEEEKSNNVWKVRFHTLTKYSDFKGASSLILSRRSVNSASSDQSKIAFHDKTDGRHQLFVLNNIPVVGRVHNCYYIFSKKDMAYIRNIIMVDSENINKLVGFCLDGPTLLSLWNYCSRGCLIDIITNDNLNINIDGFFVYSLIKDIVEGLYVIHNSAIEYHGNLSSKNCLVDERWQVKLSDYGFPFLRCLEEPKSAREQLWTAPELLRNKELRPNQSSDIYSLSIVMADLVNKNISFENSDVQKEADEIIYLLKNRNSESTRPTLNPAVENINGNLLHLIRDMWAEDPSRRPKISVIRKLINDMNETKSKNLMDHMYDLLENYAASLEEDIQHRTKELMEEKKKADLLLSRMLPKAVAEKLKLGQPIAPEHFDSVTIFFSDVVSFTTLA</t>
   </si>
   <si>
@@ -702,9 +699,6 @@
     <t>MNKLLKLIFYQFFLLPFYYFVNGNENILNVKDIIKSFQIPSYQNFTPFPYNNLTIKVGVLIPEDNEQISNTIGYHKTASGITIGYYNLIDAGFIDKNKLNFDFFFNKINCEELYATKIAIEMLTSNKVDVIFCPPCKKLANFISIISTVYNRPVYLWGTTIDSFITTTSEIQTVISTSISSLDYTYGIIEIIQYFQWKYVGFIYMVTTSDNTCLEIQRDFITTTLANTNITIQYVIEINSTTSSIKNILNEIKNLARIIIVCIPTDIYKRKFMLTVYDEGMANDEYLYILLGTNNSVSQNNNNSTALWESQEILNDNRDDDALEAFKYVFIMNKDGKNPKTNINDFSNKIKRYMIEWPVNCNDTICLNNINNSNFEASSYSYYLTDVMMLYGISLNKTLSTEPLKYNDGMLIKNNSLHVMDGYSGTLRMDTDGVKLGYFNLITYNNSRDTVNLLKIYEKNNDKYVIEILLENEDEIWFNRLNKIKPNDEPQCGFKNNKCQLSFIQQYSIYLIILIVIFVILIIGAIILIVYIRNSKRKQQQLLNNMWLIKYEDLQLINLKKIRSGRTLSSTKSIEKSLDNFKLQNTNETININNDDPLENENKRFIGYIYKEEFVVGEKFRKFLDINDKICAHLRFLREIDHENLNKFIGLTEHRKYIISIWGYCTRRSLKDWIINNKNDLEPFYIVSLMNDIASGILFLHTSSIGYHGRLTPSNCLLDNHFQVKITNFGLNFISEFYQRTEYEQLYTAPELLRTLNLSGSKEGDVYSFAIISSELLNKAPAWFYKHEKMLIPEIILKIKNSRLGNFRPIIEDNYEEVWVKDVIRLIKDCWDEDPLRRRKIKVIKNMLKSAVKVKNINLMDYMFQKAEHYAQELEEDVKTRTRELYEEKKKCDKLLYRMMPISVVEKLKAGEAVAPEYFESATVFFSDVVSFTNLCAQCTPLQVVSLLNQLYSRFDEIIEQFDAYKVETIGDAYLVVSGIPIRNGNKHGEMIANMALEFIYALPSFKLSFLPDYRLNLRIGLHTGPVVAGVVGLQMPRYCLFGDTVNTASRMESNGMPGCIHISESTQKLLSSSDIFKINQRGDVLIKGKGNMFTYWLIGRENEPEKWLKEPN*</t>
   </si>
   <si>
-    <t>TAAAAGCGTTTAGTATA</t>
-  </si>
-  <si>
     <t>SRAE_2000417200.1 split 1</t>
   </si>
   <si>
@@ -715,13 +709,85 @@
   </si>
   <si>
     <t>Reverse blastp yields strong match to gcy-36, gcy-32, gcy-34, etc - this is probably a soluble GC</t>
+  </si>
+  <si>
+    <t>Match is very short fragment. Blastp matches a Ce gene enriched in body wall muscle cells? Protein doesn't appear to have a cyclic nucleotide domain</t>
+  </si>
+  <si>
+    <t>Match is only 29 bp/AA; protein has cadherin-like domains, no cyclic nucleotides</t>
+  </si>
+  <si>
+    <t>Pulled up as homolog to SRAE_1000121200, which was a spurrious result</t>
+  </si>
+  <si>
+    <t>Has a GC domain. But the majority of this gene is missing b/c it's on a contig that cuts off at the 5' end of the gene</t>
+  </si>
+  <si>
+    <t>Contig Issue</t>
+  </si>
+  <si>
+    <t>Pulled up as homolog to SRAE_2000225200, which was a spurrious result</t>
+  </si>
+  <si>
+    <t>Contig issue</t>
+  </si>
+  <si>
+    <t>This is too short b/c the contig cuts off at the 3' end</t>
+  </si>
+  <si>
+    <t>Homolog to SRAE_2000349200, likely soluble GC</t>
+  </si>
+  <si>
+    <t>Matches to SRAE_2000448400, likely soluble GC</t>
+  </si>
+  <si>
+    <t>Contig cuts off at the 3' end</t>
+  </si>
+  <si>
+    <t>Homolog to SRAE_2000041800, which also didn't have a cyclase domain</t>
+  </si>
+  <si>
+    <t>Contig cuts off at both ends</t>
+  </si>
+  <si>
+    <t>MLYYFKYIIILYLSIFAHSKTDISLGFLFPRNSTLLESTSGFVRSAGVVTLVFEKIKKESILPDYNYDFNVFYDECDEYRATSGTYELIKYHNVDVIFGSTCNAASIRSTLMAKFYNKPTFVWGAVSSSDIAHRNRLPNIFSIFPIFLSLAYATIDVLEQFNWTTISVIYNSNPVKRCKNLFTDFEHTLTLTNTKVRIVYSLQTSFEPTPNEFDDYFFEVKDKARIIVSCFDNFKYKRKFLISMYENGLNNNEWVHINMDYRNLGFFTNIEDSLGNYSPFYKDVYDNPPDGKDDIAFEMAKKMLSVDMSTKLALSSIDDSEILENVKKWPFYCEDCNISSNTTLSTYAWYLYDAIYFWAFLINKTLPLYGDKIFNNYTLLYNHCPGNYNGMTGEINFGNTCVRAPFIILRGLDDNEETPGYITYNFSSISDYFKNVVVENFQEIMFKNWDNQIPLNVPICGYRGNLCPIDIFKDYLTEVIIVAVIITLLFLFIVFLIIFLLWRTNRKKEEEMSRWIIPYISLTKPVPEKKEYEKSLNSLASNTYSFSSKKTFNNMNETNKYIFAYLNGEGVAGEKHKNLFQTSKNDKIELSKLIKWEHDNNLLQTDNSIFDGFFLTSLIKDLSEGLNYIHNSYLKFHGRLTSKNCFINDRWQLKISNFNSFKFRCYEKLESKNLLWTAPEILRSESFFGSQEGDIYSFAIICSEIVTKKLPWDYNNRNESIEELIYLLKKSGLNTLRPDIIIAPNIDIDMTYITLIRDCWSEDCNKRPTIKQILHLLRSLKNKKANNLMDHVFGILEEYSSTLRQEISERTREIDEEQKKTDLLLSKMLPSAVAQNLKKGKIIEPENFEMVTIFFADIVKFTDLSLKCSPMQLITLINELFTMFDNLIESYDVYKVETIGDGYLCVSGLPIRNNNHAEIISDLSINFMDICKSFTIPHLGREKINLRIGCNSGPCVAGVVGLTMPRYCLFGDTVNTASRMESNSRSGRIHIAESTFKLLNDTNKYDLECRGEIIIKGKGVMTTYWLNGYKNN*</t>
+  </si>
+  <si>
+    <t>Ostensibly matches SRAE_2000427000, which is 1076 aa, with 7 exons, lots of small introns. I tried to shift around the exon to get a longer ORF for exon 2, although given the RNAseq data I'm not convinced this is accurate. However, the new protein is longer, and matched via Blastp to Ce-gcy-5, 7, 17, 14, etc... tblastn of protein back to S. ratti genome got me ,matches to SRAE_X000000200 and SRAE_2000494300, neither of which previously had a S. stercoralis homolog listed</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Ss</t>
+  </si>
+  <si>
+    <t>Sr</t>
+  </si>
+  <si>
+    <t>Too long</t>
+  </si>
+  <si>
+    <t>Looks like there is a gene with a zinc finger domain here at the 3' end. Protein kinase domain and TMHMM earlier in the sequence, around 1300 is where the trouble starts.</t>
+  </si>
+  <si>
+    <t>Two protein kinase domains - one at 530-800, another at 1570-1840. I suspect this is two genes. Also too many TMHMM regions</t>
+  </si>
+  <si>
+    <t>This has lots of zinc fingers in it, no cyclase domains. Seems unlikely to be a real hit. This "matches" to SRAE_1000175800, which had two genes in it that needed to be split</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Yes?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -749,6 +815,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -778,11 +850,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1100,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD26190-B7C4-5541-9406-924BAE3C096B}">
   <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="Y11" sqref="Y11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1523,7 +1601,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>
@@ -1547,7 +1625,7 @@
         <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K6" t="s">
         <v>21</v>
@@ -1612,7 +1690,7 @@
         <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F7" t="s">
         <v>31</v>
@@ -1746,7 +1824,7 @@
         <v>18</v>
       </c>
       <c r="W8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="X8" t="s">
         <v>22</v>
@@ -1992,7 +2070,7 @@
         <v>33</v>
       </c>
       <c r="Y11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
@@ -2605,7 +2683,7 @@
         <v>35</v>
       </c>
       <c r="H25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I25" t="s">
         <v>35</v>
@@ -2625,7 +2703,7 @@
         <v>33</v>
       </c>
       <c r="E26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F26" t="s">
         <v>25</v>
@@ -2675,8 +2753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4AF0C57-95CB-A24A-8D1E-C9EDB24C1D1D}">
   <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3186,7 +3264,7 @@
         <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D7" t="s">
         <v>49</v>
@@ -4392,7 +4470,7 @@
         <v>72</v>
       </c>
       <c r="L22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M22" t="s">
         <v>69</v>
@@ -4448,7 +4526,7 @@
         <v>67</v>
       </c>
       <c r="I23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J23" t="s">
         <v>73</v>
@@ -4663,7 +4741,7 @@
         <v>73</v>
       </c>
       <c r="U27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
@@ -5162,7 +5240,7 @@
   <dimension ref="A1:A55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5189,7 +5267,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
@@ -5204,7 +5282,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
@@ -5264,7 +5342,7 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
@@ -5284,17 +5362,17 @@
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
@@ -5324,7 +5402,7 @@
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
@@ -5349,743 +5427,1018 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{427D24AC-C616-B842-8203-23EFB599A2A4}">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="34.83203125" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" customWidth="1"/>
-    <col min="5" max="5" width="47.83203125" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" customWidth="1"/>
+    <col min="6" max="6" width="47.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" s="2">
+        <v>462</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E3" s="2">
+        <v>255</v>
+      </c>
+      <c r="F3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" s="2">
+        <v>178</v>
+      </c>
+      <c r="F4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E5" s="2">
+        <v>160</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>216</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B6" t="s">
+        <v>241</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E6" s="2">
+        <v>715</v>
+      </c>
+      <c r="F6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E7" s="2">
+        <v>698</v>
+      </c>
+      <c r="F7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="E8" s="7">
+        <v>581</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B9" t="s">
+        <v>241</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="E9" s="7">
+        <v>332</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" t="s">
+        <v>241</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
+      <c r="D10" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E10" s="2">
+        <v>231</v>
+      </c>
+      <c r="F10" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>216</v>
+      </c>
+      <c r="B11" t="s">
+        <v>240</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E11" s="2">
+        <v>548</v>
+      </c>
+      <c r="F11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>216</v>
+      </c>
+      <c r="B12" t="s">
+        <v>240</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E12" s="2">
+        <v>245</v>
+      </c>
+      <c r="F12" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E13" s="4">
+        <v>2877</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" s="4">
+        <v>2095</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>241</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>241</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>241</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>241</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1120</v>
+      </c>
+      <c r="F18" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>241</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>241</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D20" t="s">
+        <v>219</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1113</v>
+      </c>
+      <c r="F20" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>241</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>241</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>241</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>241</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>241</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>241</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>241</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>241</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>241</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E29" s="2">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>241</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E30" s="2">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>241</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E31" s="2">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>241</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E32" s="2">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>241</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E33" s="2">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>241</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E34" s="2">
         <v>1027</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D4" s="2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>216</v>
+      </c>
+      <c r="B35" t="s">
+        <v>240</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E35" s="2">
+        <v>1778</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>246</v>
+      </c>
+      <c r="B36" t="s">
+        <v>240</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E36" s="2">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>240</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E37" s="2">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>240</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E38" s="2">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>240</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E39" s="2">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>240</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E40" s="2">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>240</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E41" s="2">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>240</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E42" s="2">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>240</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E43" s="2">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>240</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E44" s="2">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>240</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E45" s="2">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>240</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E46" s="2">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>240</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E47" s="2">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>240</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E48" s="2">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>240</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E49" s="2">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>240</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E50" s="2">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>240</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E51" s="2">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>240</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E52" s="2">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>240</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E53" s="2">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>240</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E54" s="2">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>240</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E55" s="2">
         <v>1059</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>217</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D5" s="2">
-        <v>231</v>
-      </c>
-      <c r="E5" t="s">
-        <v>215</v>
-      </c>
-      <c r="I5" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1120</v>
-      </c>
-      <c r="E6" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C7" t="s">
-        <v>220</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1113</v>
-      </c>
-      <c r="E7" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D9" s="2">
-        <v>698</v>
-      </c>
-      <c r="E9" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D10" s="2">
-        <v>1077</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D11" s="2">
-        <v>715</v>
-      </c>
-      <c r="E11" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D12" s="2">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1099</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D14" s="2">
-        <v>1128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D15" s="2">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D16" s="2">
-        <v>1061</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D17" s="2">
-        <v>1518</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D18" s="2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>240</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E56" s="2">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>240</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E57" s="2">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>240</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E58" s="2">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>247</v>
+      </c>
+      <c r="B59" t="s">
+        <v>240</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E59" s="2">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>240</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E60" s="2">
+        <v>686</v>
+      </c>
+      <c r="F60" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>240</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E61" s="2">
+        <v>678</v>
+      </c>
+      <c r="F61" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>240</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D62" t="s">
+        <v>237</v>
+      </c>
+      <c r="E62" s="2">
+        <v>642</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>240</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E63" s="2">
         <v>332</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D19" s="2">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D20" s="2">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D21" s="2">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D22" s="2">
-        <v>1522</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D23" s="2">
-        <v>2877</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D24" s="2">
-        <v>1060</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D25" s="2">
-        <v>1060</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D26" s="2">
-        <v>1064</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D27" s="2">
-        <v>2095</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D28" s="2">
-        <v>1120</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D29" s="2">
-        <v>1135</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D30" s="2">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="D31" s="2">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D32" s="2">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D33" s="2">
-        <v>1059</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="D34" s="2">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D35" s="2">
-        <v>1153</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D36" s="2">
-        <v>1079</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D37" s="2">
-        <v>1129</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D38" s="2">
-        <v>1065</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="D39" s="2">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B40" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="D40" s="2">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D41" s="2">
-        <v>1104</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B42" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D42" s="2">
-        <v>1088</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B43" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D43" s="2">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B44" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D44" s="2">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B45" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="D45" s="2">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B46" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D46" s="2">
-        <v>1060</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B47" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D47" s="2">
-        <v>1062</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B48" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D48" s="2">
-        <v>1076</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B49" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D49" s="2">
-        <v>1056</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B50" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D50" s="2">
-        <v>1070</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B51" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D51" s="2">
-        <v>1033</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B52" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D52" s="2">
-        <v>1117</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B53" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D53" s="2">
-        <v>1069</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B54" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D54" s="2">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B55" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D55" s="2">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B56" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D56" s="2">
-        <v>1134</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B57" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D57" s="2">
-        <v>1085</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B58" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D58" s="2">
-        <v>1062</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B59" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="D59" s="2">
-        <v>1055</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B60" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D60" s="2">
-        <v>1503</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B61" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D61" s="2">
-        <v>1222</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B62" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D62" s="2">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B63" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D63" s="2">
-        <v>1778</v>
+      <c r="F63" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D55">
-    <sortCondition ref="B1:B55"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F63">
+    <sortCondition ref="A2:A63"/>
+    <sortCondition ref="B2:B63"/>
+    <sortCondition descending="1" ref="E2:E63"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating with better gene models
</commit_message>
<xml_diff>
--- a/Code/rGC Homology/Ce-rGC_tBlastn.xlsx
+++ b/Code/rGC Homology/Ce-rGC_tBlastn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astrasb/Documents/RStudio/Bryant_et_al_2021/Code/rGC Homology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96A9710-BA0A-B144-B5BD-E229A478CC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EACAE19-ACB2-9946-8336-08A6695D6868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="6200" windowWidth="34900" windowHeight="16200" activeTab="5" xr2:uid="{AD4C77C0-16BB-4E4E-91C7-9E778F091754}"/>
+    <workbookView xWindow="780" yWindow="1060" windowWidth="26420" windowHeight="15260" activeTab="5" xr2:uid="{AD4C77C0-16BB-4E4E-91C7-9E778F091754}"/>
   </bookViews>
   <sheets>
     <sheet name="Ce_to_Sr" sheetId="2" r:id="rId1"/>
@@ -20,24 +20,17 @@
     <sheet name="Homologs" sheetId="6" r:id="rId5"/>
     <sheet name="Sequences" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1585" uniqueCount="287">
   <si>
     <t>DAF-11</t>
   </si>
@@ -279,9 +272,6 @@
     <t>SRAE_1000114200.1</t>
   </si>
   <si>
-    <t>SRAE_1000137800.1</t>
-  </si>
-  <si>
     <t>SRAE_2000024700.1</t>
   </si>
   <si>
@@ -294,9 +284,6 @@
     <t>SRAE_2000427200.1</t>
   </si>
   <si>
-    <t>SRAE_2000430600.1</t>
-  </si>
-  <si>
     <t>SRAE_2000431000.1</t>
   </si>
   <si>
@@ -333,9 +320,6 @@
     <t>SSTP_0000210000.1</t>
   </si>
   <si>
-    <t>SSTP_0000214200.1</t>
-  </si>
-  <si>
     <t>SSTP_0000214300.1</t>
   </si>
   <si>
@@ -351,9 +335,6 @@
     <t>SSTP_0000354300.1</t>
   </si>
   <si>
-    <t>SSTP_0000489700.1</t>
-  </si>
-  <si>
     <t>SSTP_0000664100.1</t>
   </si>
   <si>
@@ -369,12 +350,6 @@
     <t>SSTP_0000817800.1</t>
   </si>
   <si>
-    <t>SSTP_0000846800.1</t>
-  </si>
-  <si>
-    <t>SSTP_0000912800.1</t>
-  </si>
-  <si>
     <t>SSTP_0000937800.1</t>
   </si>
   <si>
@@ -405,9 +380,6 @@
     <t>SSTP_0001276100.1</t>
   </si>
   <si>
-    <t>SSTP_0001276100.2</t>
-  </si>
-  <si>
     <t>SSTP_0001276200.1</t>
   </si>
   <si>
@@ -435,18 +407,9 @@
     <t>MNILKLFFLVILSLSINGQKNLNLGFIFVKTDSENGDILGFTLAVGIIPVVIDRITSEKLLPQYNFTFNYYFDDCIEKNSSGLTYQLIVNDKVDVIFGPSCSINAIRASMIAKFYNKPIFIWGLVSSTQFTNVKRFPNVYSVAPVFYSLALTVLDILKTFNWHKYVFFSCSRLNNRCNMMFDDFVNAANIFDFKAVMVYSYKASTPPLDIEYDAFINETIIRARIIITCFDRNDWKRSFLLKMYDRGLNNSEYVHINMEDTSKAFNSHYVDSNDNPIPFYNDVDKNNDGRDMDAFEMAKRMFIFDTAKYYNTNKSFDKEVIKRVNDWPFYCNVCNINDSTILNRYARYLGDSVYIWATLLNKTLDEFSEKTFENPTLFRKQCLLSKEGYTGIINFDSNCIRLPTIQVTGLDKFGKQIVWFNYSYTSLTSFKKESSVSLNNFPKTIFENWNNSIPLTEPICGYLHNRCQKNFFKFYFKEVIIVGVIILILILFIIIGLIWYICKVKVRKGEELNKWKISLSNLISDVTNNDATESIHSSVSEITTNTFKFNLQKKNNTENYSFYLYNDEEVVGRKYKNIFNYTNNDCLQLNKIISINHENLNKFFGICIDGTLPISVWKYCKRGSLHEILQTDIPNFDSYFMMSLTKDIYNGLSYIHSSFINFHGTLNSKICFVSDRWQVKISNFSTKQLSAYDKTNIENLLWRAPEHLTHDFSIGSKEGDIYSFGIILSEIISKGNFWNLSSRQESVEELIYLLKRGNSNDLRPEIIVAPNVEVNPSFITLIKDCWNYDDKKRPNIKQIEKLLNVFTKKNAKNLMDHVFKILEKYSLTLQDEINDRTKEIVEEQKKSDILLKKMLPAEIVEKLKLGKTVEPENYDNVTVFFADIVKFTILSSKCSAFQVVTLVNDLFILFDNLIESLDIYKVETIGDGYLCVSGLPTRNGDMHGKQIAELSLGFNEICHKFSIPYLPGEKIMVRIGCNSGPCVAGVVGLAMPRYCLFGDTVNTASRMESNGKPERIHITESCSKLLNKIGGYVIEPRGEVIIKGKGVMNTFWLNGRIGENNNHMIKNDEVKFEPILNLDEKKTNTNMGMYREFGKNNN*</t>
   </si>
   <si>
-    <t>MSSPNPRYSIQRIKGYYNNVGAIHNPEVVLSSYNNGSRQMTLNDRFNFLRRGYNIYELKKARESQRNYTVTLTHNFADVFNFVFIINGINVTFLRNDGNTTIACTTAIEHAKSSGQCQDDIYLKIGDACRIGNDALGTVAACDFFYNENAKAIVGPECFDESSHLALLSYHWKIPLFSPNGKVVYNYNNTVFPTVIHTSFSNVVLYANSLMLFMNRFNLSSVTFLGPKDDRNIHFRSIFEGVNKYFKTYFYNITTNIISIEESRLSSYNPKDIGLISFIKLIVIDTSFNDLHSVLQQMEVSSLYDHGYIFILLCSQHSSVCDSNIDKIILDCNMLLLGPYFKNYTDIDLLMSQYFKDSYNRFKGINYLSTYISCYSSCVASKLNTNLDGTSVVNTMKGKQLNTSLGNFIFDQMPSILITQSFSQYDSVNNTFVDLILTNPIASTCSKNKCFNLEIKVNNDEFWKSQLASPLTHCHLFKNCTNYLVIILCVTGAVVLIIILILIYMLRRQRRLNVYRMNWKIPKSQFKVIENKVSNSKKQGNTAETLSSKRRYIHAYAIVDTTKAEFLQLRQLKKIVWSKPEIKFITELKKISHDNLTNFLGVNYNDTDKFYMLSSLIDRASLEDLVDDTDFNLDMTFKSAFIRDILKGLQYLHKSFIGYHGLLNIQTCLIDANWVLKLSNFGITNILHNLIHDEVLKNIELINLHFYQTISPENLQGCNFGINYPMGSQNGDIYSFGIILYRLTYRHGPFDHVSMVPKDILKEIVKNTIEPTFDETLEDNSLLDLMKNCLKFNHLERPSLKVLESSITTILHSTRGNLVDQMINMNEKYAQNLEKVIAERTNMLVEAQLQTDRLLSEMLPRSIAETLKNGGTVEPKLYESATVCFVQICDFAKFMEENLPPAVMSFLNDIFNMFDDVIHNYDCYKVETIGDTYMVVSGVPKENEGKHVFVIAEVAISLRSHSLHYDVPVKPDWKLQVRIGFHCGPIAAGVIGLKAPRYCLFGDTVNFASRMESNCPANQIQVSESTALKLMENPEYRLIKRGIVKVKGKGDVNTYWLNEHFHQNEILSASKS*</t>
-  </si>
-  <si>
     <t>MFFPFNNTNQLKWQGYQNSAGAVLEAFKLAKTNYTALNDIDVTYKWLYNECVMSTAMGNFFEMITSENDSIDVMFGPACSETATLCGSIATYYNFPIFLYGLSSVFSSFEDTSLYPTVVAVMPIYKDGARALTNILLNYEWTDISLVYINSIEMLRRCEKFANEFDSYISSDINNIDIVYKKLISNFSSSNLANIAKTISTVSRIIVICIGEQEKIRKLMLAFYDNGMNNDEYVYINCDVDMDIYVNSENILLLKDYNIPPDGRDNDLFSMYTYMLHFQYYITGGLSDSYNDLRLNMPKYMAQPPFNCTTECEMFNVSSIYAPYLFDAAYVYYACLAKAIDDNNDKKPFKDIARDGKLIANYSTNTFQGITGEFSINSYYIRNTLMSLGTYFNDGLNVTNWVEVNVVEGKSELKLLYTDPTTSIWKIRGGKKPLNEPECGYTNTKCPYKFIQENPVAFGFIIFGGVIIITIIILIFIYFYIQKKRQEEKQNDMWKINYQSLTKYEDYEKSLSLEQSKKSITSSTNVSTKLLTKYNPEGRHRLYVYNNEYVMARLHDCFYMLTKKDMAHLRSLRMLDHDNVNKIIGFSLNGPALMSIWKFCSRGSLVDILTNDNLNINIDGFFIYSLIKDTVEGLYFIHHSVIEVHGNLSSRNCLINERWQVKLSDYGLPFLRIFEENKQEYLLWTAPEVLRFDISYPNKESDIYSLSIVLADLINKGISFDNDDVRGGAEEVIYLLKNKKSNPFRPNLDPAVEDIPSAMLHLIRDMWAEDPSIRPKIDVIRKLVKQMKIGKSSNLMDHVYSMLENYAASLEEDIQSRTKELVEEKKKADLLLSRMLPKAVAEKLKAGQTIQPEHFDSVTIFFSDIVSFTTLASKCSALQVVDLMNGLYTMFDSIINEHDVYKVETIGDGYLCVSGLPERNGNRHIKEIANLSLELLKQIPGFRIDHLPNEKIRIRIGIHSGPCVAGVVGLTMPRYCLFGDTVNTASRMESNGKPNHIHMSNDAHKLLTEKIGGFVTEPRGEVLIKGKGVMETFWLIGKVGEVSTNSTNGMYTDYKKEPE*</t>
   </si>
   <si>
-    <t>MLLKILSLILLFNLITGQQTNTTLAANLLNTTKVMKSFNIPSYSERTPFPFNGSINVNVGFLISKGDADYEDTVGYYKTASAIMIGLEELIHAGFIDTTKVQFKFYFRFSNCSVLQGTKTTIELLQNDNVDVFFAVACQELSDFISVISTSYGTPLYLWGPPISTYIVNSNEKRSVISTSISIEDYSNSVKSLVDYFEWKKISIIYMTTTLHSVCGNMQTNLINTVLTTTKTVVVYSGSVNSSGDSMVENLLAISNVSRIVIVCIPSNDLKRKFMLTAYDMGMTNDEYVYLIIDVNDTVIENSDDSIPVWKDSSNLQDDRDEDALEAFKFALLIDKTAENNVDMKRFARNISKGMLDYPFYCNETECLKNSKDPNFHYSTYAPYLADTMILFGLALNRTLSTTPLLYTDKDILKNNSAYSFEGFSGNVVLDNNTVRYGYFFVRYIGNDSKIYTNMIITRNKNQTYYVHSYGTSNENKMWWNRKDFSRPLDTPLCSFAGNKCPKTFWEEYFIIIIIVIITFIGILIFSIIVIILLRRYRIRQQRQLDMLWLINYEDLKSIKSNERMYGKSVISINDSQKTLNKDIEILNNKDNELNLNERDNRRHIVYRYNDETVVGEKFPKSITITSAERNHLRMLRNIDHECLNKFVGLTESPTHVIGVWKFCVRGNLKDLLKNKVREIDPYFVVALMNDISSGIQYIHSSKINCHGRLTSSCCLLDSNYQIKLSDFGLSFLRKYIKRNFEEQLYTSPELLRSQNVLGTKEGDIYSFAIISSELLNKSLEWPEDEISHTKNDIITKIKNSRRGTFRPIISYEVKERWVGKVINIIKDCWDEDPLKRKKIELVRKMIKSSMNNKKISMMDYMFNKMENYASHLESEVMGRTKELMEEKKKSDILLYRMIPKSIADELKSGRTVAPEYFESATVFFSDVVSFTNLCAQSTPLQVVSFLNQLYSQFDEIIERFDAYKVETIGDAYLVVSGIPIRNGNKHGEMIANMALEFMKALPLFKLSYFPDYRLNLRIGLHTGPVVAGVVGLQMPRYCLFGDTVNTASRMESNGMPGCIHISSEMCELLTQFDTFEIENRGEVMIKGKDIIKSFQIPSYQNFTPFPYNNLTIKVGVLIPEDNEQISNTIGYHKTASGITIGYYNLIDAGFIDKNKLNFDFFFNKINCEELYATKIAIEMLTSNKVDVIFCPPCKKLANFISIISTVYNRPVYLWGTTIDSFITTTSEIQTVISTSISSLDYTYGIIEIIQYFQWKYVGFIYMVTTSDNTCLEIQRDFITTTLANTNITIQYVIEINSTTSSIKNILNEIKNLARIIIVCIPTDIYKRKFMLTVYDEGTNNSVSQNNNNSTALWESQEILNDNRDDDALEAFKYVFIMNKDGKNPKTNINDFSNKIKRYMIEWPVNCNDTICLNNINNSNFEASSYSYYLTDVMMLYGISLNKTLSTEPLKYNDGMLIKNNSLHVMDGYSGTLRMDTDGVKLGYFNLITYNNSRDTVNLLKIYEKNNDKYVIEILLENEDEIWFNRLNKIKPNDEPQCGFKNNKCQLSFIQQYSIYLIILIVIFVILIIGAIILIVYIRNSKRKQQQLLNNMWLIKYEDLQLINLKKIRSGRTLSSTKSIEKSLDNFKLQNTNETININNDDPLENENKRFIGYIYKEEFVVGEKFRKFLDINDKICAHLRFLREIDHENLNKFIGLTEHRKYIISIWGYCTRRSLKDWIINNKNDLEPFYIVSLMNDIASGILFLHTSSIGYHGRLTPSNCLLDNHFQVKITNFGLNFISEFYQRTEYEQLYTAPELLRTLNLSGSKEGDVYSFAIISSELLNKAPAWFYKHEKMLIPEIILKIKNSRLGNFRPIIEDNYEEVWVKDVIRLIKDCWDEDPLRRRKIKVIKNMLKSAVKVKNINLMDYMFQKAEHYAQELEEDVKTRTRELYEEKKKCDKLLYRMMPISVVEKLKAGEAVAPEYFESATVFFSDVVSFTNLCAQCTPLQVVSLLNQLYSRFDEIIEQFDAYKVETIGDAYLVVSGIPIRNGNKHGEMIANMALEFIYALPSFKLSFLPDYRLNLRIGLHTGPVVAGVVGLQMPRYCLFGDTVNTASRMESNGMPGCIHISESTQKLLSSSDIFKINQRGDVLIKGKGNMFTYWLIGRENEPEKWLKEPN*</t>
-  </si>
-  <si>
-    <t>MIDNKIFSFFIFIFYFKLLYSSSTTEIPIVLSTIINDNKTTNVTNNDLNKSENMSNVLSGSTIRKGKGKIVRIGHIGALNAMPNAELVLDMARKELWRDGILDDEFDVELINTRACGESFEGVAVAADMFHLQDVKAFIGPYCNAEMDAVSKMAAYWNVPIIGYMAASNTFSDKTIYKTLARVSIRTTNSLAYAVATTLKHYNWKNVAIVTNTGVVALERTVSFEENFHKLGINILRKITFDENADTKLILESGLMQDIKNTARIIICIFTKTRDMTIEFMKAVVQAKMNTNDYVYIFPWLQAEAKEPPPWIDKEGHINTNIKKIFSNSIIVDDINGFDNTLTTPFVEKMEKNNLDINELDLSNVYGYIHLYDSLKLYSLIVRSIMNKTGGDFDPLTNGKKIWNEMRRFSFPGLVSIEGTSAGNVIMDDLAERAASYGAFYINPDRDDVIKMVEMEPVFVNNCDGLKTKSGCYELKVSDIVTGFWPSPDGKLPFDIPNCGLSISRILENRALANTPWRIWRDDTRTITEDEMKSMLSIGSSKTKISNMSKFVKHHAVIGTNTHASYHIYPQKRLITFAREDIKLLNQMKLLVHDNLNPFLGMSFNEKDEMLLYWKFCSRGTVQDIIYNDDINIDSNFHAAFIRDITAGLEYIHLSPVIFHGSLTPWACLIDRNWTVKLTDYTIASLVEKWTKLSMIDPEAIKDGENKAAATQKSYVLYCSPETLKTSETNKRKNNESDWVKQSGSRKQASDIYSFGIVMYEILYRSLPFSDTLNVDELIDGNKLGNANIKPSIQDRSKIHPDLCALLLDCWNINPEVRPSIKRVRLNTEHYLKVKGSLVDQMMRVMEQYANNLEKLVQERTGMLEEANIRADKLLSQLLPSYIANELKMGKSVPPKLFEQASVMFSDIVGFTKICSSSSPLEVVNFLNSVYTGFDDIINKHDAYKVETIGDAYMVVSGIPQENGVNHLANLADVTLCMMEFLQTYIIPHKKNEKLRIRLGIHCGPVAAGVVGLTAPRYCLFGDTVNTASRMESTGLPEQIQISTFFNDRLNKHFPEFDTSLRGPVLVKGKGEINTYWLEGKNGRSITAPIPVELQNQFGKI*</t>
-  </si>
-  <si>
     <t>MINNKKLYGIIDEKDKNIIYRKQRNTESSISSQGKKIITISYLSAISVFPRNLYDYIKTVTNSSNSNNLFKKKSDKLDIFSNYNYVSKCFKADFDGSLISGALKFAIDEINSNENLLPDYYIKYVFNNTCDDETLSTKYFMDHWKSGVSAFIGPEMNCRTEAQMAAAQNLPIIAYKCKDEVVSNKLKYPTFARTVPAESAIAKTVVATLKEMNWKKVALIYEEATSYSKLVDSIKLIIEQQNRHLKVNNKYEILSINTIPSPFSEFNDNKFDQIVGETKDYSRIYLVVGTPKMGRKLTKVMGDKNILSSGLYLILLVCPDYDWLNTYHAMNNHFFRDTSKWLSKSWDVNNSDDHKFLTYAQYVLAIIPTPVSLNNPQVKFFWKKCNENLKYFGIYGNPFEKEIKPNRHAYYLYDAVMLYAKSLHEVVKYYKKNGFNTDLAIKDGRMIMSHIIGKRYFSIQGFEMKINKNGNAIGNYSLISLQKVEPIYDKNNPNYYPIKYALDVTADFVDVDDGLLTLPKMRYHKKILWPRTSPPIDEPICGFMDDKCSVNIFLKYIWAFFFFFFFCLLGSYLGFKHYYEKKLRLEEIPNTWKIDIKKIEKISKNNDTFKSLLFFDEDSGIFSDEFTKILARYIPKSTFKKNKSLECGNQKFSKLSGIGLYEGSFVVVKEFTYDHDRKIISDSLKKECNVMKQLRNDNINNFLGLLVGPYSIYAVREFCGRCSLMDVYKNNDFKLDNLFISSFIDDLVKGMLYLQNTEIKIHGNLKSTNCLITNRFALQLSDFGLYELRYGQDFKTEELMWEGLLWTAPELINFDDVARPKPGTQEGDVYSFGIILHELVTGDGPFRLLSKNNICAAEIIKNIVEDDNFRPDTKFLNCPKFVIKCMKECWQKCPKLRPTFQNGIRQLLLPMLEQVMKNNLMDNMMALMDVYQNQLEDLVERRTLQLQNEKRKSEALLQRMLPPSVANQLIKDGKVRPEFYKSVTIYFSDIVGFTDLANFSTPIEIVSFLNDLYTMFDSIIKKYEVYKVETIGDAYMVVAGCPKYYSAIKQAEEIASMALHILACSSTFVIKHKKNEKLSIRIGIHSGCVAAGVVGKTMPRYCLFGDTVNTASRMETTGSGMKIHCSIDTRSLLESKENFLFEHRGFQYIKGKKPVLTYWLLGRLDWKEDVYYYIDSKSDDLNNSKSCFIKNYNKNREKLPLKYNDDNNSIFSNISLYKIKYFMNQPKSNCEYEFLNEEYNIVESLKNSHSSEELSLYECRNNYEKVFKKTKANLLKKSLSFPILKVKKPWNDKKINSFRKLTKKSTTISTMSILESVFSDEDYNNDDSRNLIIEDDSLDYDDDSDYTYENSDSETSSMSSLMEYRNFSYNDNDILKNNGFKDNKIIKRVKSINYDSCKGISKYFRNPTFVEYKSLSKNSSFDEGYMDRYAVNKSILNDYNEYDLEAAKSWNNSTTKNSYFPVHRNRKSGIVRNGRNNKDSQETNSFKESLITKALSIFNQRKGIRKNKKSNLFINEGDLTD*</t>
   </si>
   <si>
@@ -492,30 +455,18 @@
     <t>MYFYDKIFYDYIKLIVCSGKFNISLNSRYFLICYFFIFLSTVFIIPQTIFEEPTHAKPLAMNVGVIYDDKWANNIKTFLSTVINNIYNENSSLIFTINPIFSSKIPQCKNIIGSGEGAYILSQIYYSNQNKNSNIGGVETFIGPTCSSDLRIASRISKQLNLLEFNIWNEYVNEAFDNEIVQMSTESGTNIALNLYTVLTRLNWKQVALLYCSECMFKFNGNILVNEEDLTLQTIMNVLKANYIIVTECIVVKKQDMNNSIYMKKLLQELKTKTRIIVPIFGASLNNYKAYMEAAKENDMKTNKYMTIIFKFFEFPKSPEPWITTNGSINEDILKLYDRTIVLKNDYYLEEQINAFEKKYSLQVTDNSILFYLQLYETIFTFMFMITKAYAHSSNNISLFSSSEYSSYLMEYIRNNKIDGPYGPIYFDNSNQRVAPYKIEAIEYSTTVKGYNKFIDININEICISEDVDPSYSKNCPALIAYITNTDAHILEDLPQDMPSCGFDGELCDQTGTIIIIVAVIITVILVTLIFIFVRRMRTGETANMPWAIEPEDLEIFEDNSHLIGSSGGFQSNVSIHSMHQQFGSKVKMRELLRNCLVGKIKGTGTVFVEPYQLKEKMVYDKQDMQLLFTLRQTIHDNINPFIGICMDNKRNEFSFIWQCALRGNLSSMLFSQQDKIIRDVDIGKDFTGAFVRDILKALDYIHSSSLQYHGGLTPSNCWIDSHWILKIGGCCTARMLFKWKSHGILAGKKDFPIILNSDLHYYAPELRKAIRNNMHTNKIEKLEFSNADGQKQDIYSFGIILYEMLFKKKVVEIDDSYGMQNNDEDFGIFNTQAEALIPLYPTIPENHDDVHPDLISLMHKCYNGNASLRPDSNMARKITDATLKMPGSLVDQMIKNLEQYTNNLENLIEERTGELEREQKRAEQILLDLIPKSVADDIKLGRKIEAKTYKYCTIMNSDIVGFTSLCSGILPMEVVNLLSGLAKNFDRIITDNKCFKIETIGDAYVVSCGLPEPSRYNNVKNIANMTLQMREFLLSYKVPHRPEKHLQCRFGFNSGPVFSGVIGLKAPRFCVFGQTASIASKMEQNGVPDHIQMTLRSYQLLEGKFPEFICVPRGGIRIEGIGTLLTYFLEGKDLSKIRTDLVPWDDTDIDN*</t>
   </si>
   <si>
-    <t>MYFYDKIFYDYIKLIVCSGKFNISLNSRYFLICYFFIFLSTVFIIPQTIFEEPTHAKPLAMNVGVIYDDKWANNIKTFLSTVINNIYNENSSLIFTINPIFSSKIPQCKNIIGSGEGAYILSQIYYSNQNKNSNIGGVETFIGPTCSSDLRIASRISKQLNLLEFNIWNEYVNEAFDNEIVQMSTESGTNIALNLYTVLTRLNWKQVALLYCSECMFKFNGNILVNEEDLTLQTIMNVLKANYIIVTECIVVKKQDMNNSIYMKKLLQELKTKTRIIVPIFGASLNNYKAYMEAAKENDMKTNKYMTIIFKFFEFPKSPEPWITTNGSINEDILKLYDRTIVLKNDYYLEEQINAFEKKYSLQVTDNSILFYLQLYETIFTFMFMITKAYAHSSNNISLFSSSEYSSYLMEYIRNNKIDGPYGPIYFDNSNQRVAPYKIEAIEYSTTVKGYNKFIDININEICISEDVDPSYSKNCPALIAYITNTDAHILEDLPQDMPSCGFDGELCDQTGTIIIIVAVIITVILVTLIFIFVRRMRTGETANMPWAIEPEDLEIFEDNSHLIGSSGGFQSNVSIHSMHQQFGSKVKMRELLRNCLVGKIKGTGTVFVEPYQLKEKMVYDKQDMQLLFTLRQTIHDNINPFIGICMDNKRNEFSFIWQCALRGNLSSMLFSQQDKIIRDVDIGKDFTGAFVRDILKALDYIHSSSLQYHGGLTPSNCWIDSHWILKIGGCCTARMLFKWKSHGILAELRKAIRNNMHTNKIEKLEFSNADGQKQDIYSFGIILYEMLFKKKVVEIDDSYGMQNNDEDFGIFNTQAEALIPLYPTIPENHDDVHPDLISLMHKCYNGNASLRPDSNMARKITDATLKMPGSLVDQMIKNLEQYTNNLENLIEERTGELEREQKRAEQILLDLIPKSVADDIKLGRKIEAKTYKYCTIMNSDIVGFTSLCSGILPMEVVNLLSGLAKNFDRIITDNKCFKIETIGDAYVVSCGLPEPSRYNNVKNIANMTLQMREFLLSYKVPHRPEKHLQCRFGFNSGPVFSGVIGLKAPRFCVFGQTASIASKMEQNGVPDHIQMTLRSYQLLEGKFPEFICVPRGGIRIEGIGTLLTYFLEGKDLSKIRTDLVPWDDTDIDN*</t>
-  </si>
-  <si>
-    <t>MSAGQCQDNFFLLYGDACVVDSDALGTVKACGYFYNENAKVIVGPECYDETSHLSFLSYHWKIPLFSQSGKIWFGYNNTIYPTVIHTSFLNVVLYADSLMLFMNRFNLSSITFLGPKNEKDIHFKPLFEAVDRYFKVFYTNITTNIISIDESMLSYYNPRDIGLISFIKLIVIDTEFNDLNNVLQQMEIPTLYNHGYVFILLCSQYSSVCARPYFENYTNIDSLMRQYFRDSYNRLKGIEYLSAYISCYSSCVASKINTNLDGTSVANSMKGKQLNTLLGNYAFDQMPSILITQSFSQYNSQNNSFIDLILSKPISSNCKDNRCFSLDFIVNNDKFWQSQLASPLTHCHLFKNCTNYLVIILCVTGAVILIIILILIYMLRRQRRLNIYRMNWKIPKNQFKVIENKVSNSKNKQGNTTETLSSKRRFIHAYAIVDTTKAEFLQLRQLKKIVWSKPEIKFITELKKISHDNLTNFLGVNYNDTDKFYMLSTLVDRASLEDFVDDPDFTLDITFKSAFIRDILKGLQYLHKSYIGYHGLLNIQTCLIDANWVLKLSNFGITNILHNLIQDEVLKNIELINLHFYQTISPENLKGCNFGINYPMGSQNGDIYSFGIVLYRLTYRYGPFDNVSMVPKDILKGIVENTIEPVFDETLEDSSFLDLMKNCLKYNHLERPSLKTLESNIKTILHSTRGNLVDQMINMNEKYAQDLERVVAERTNMLVEAQQQTDRLLSEMLPPSIAETLKNSGTVEPKLYESATVCFVQICDFPKFMEENLPPAVMQFLNDVFNMFDEVIHNYDCYKVETIGDTYMVVSGVPKENEGKHVFVIAEVAISLRSHSLHFNVPVKPDWKLQVRIGFHCGPIAAGVIGIKAPRYCLFGDTVNFASRMESNCPPNQIQVSESTALKLMENPEYRLIKRGIVKVKGKGDVNTYWLNEHFHPTEDSSN*</t>
-  </si>
-  <si>
     <t>XKCTALQVVDLMNGLYTIFDSTINEHDVYKVETIGDGYLCVSGLPERNENRHITEIASLSLELIKRIPEFKITHLPNEKIRIRVGINSGPCVAGVVGLTMPRYCLFGDTVNTASRMESNGKPSHIHMSKEAHELLKNVGGFVTEPRGEVVIKGKGVMETYWLLGKIGGISINSSNEM*</t>
   </si>
   <si>
     <t>MIRIKVLLLLLSTYYLPVSTDEVPKKFTLGFLIPRTNNSLIDNGIGFERIAGAIPIAINKSKEDNIIPKDTVVDIVWYHENCDESLASGYTAKLIFENDADVIFGPACSDAAAQSGSLTTYYNFPQVFFGQTLSSELSQTNRYSTQIMISVDTGNVAYALTTFLMNFQWTQFAFFYSSLNENPLAVCTYVQSDVDLAVYAIPELSMIYKRGVNGYTDAELSTVILRMNVTARIIVTCFDEVEMQIRFLNLIPKLLDNRNEYVFIFIETWKKGFGSPLLWEISKDSSVNANVKEACKNIIIFDLQPYNSSLTSFLEDVKAAVQKEPFNCTTCANLEMSDIAASLADGIQAYFRGITRSIKAGIPNATSNGNEFMLHSAISFQGFTGMVSLNLNGTRDPTFYIYSLDDNYNSILFGTVPLVFNKSSYRPVINSDKVIFQNWGGSRPPAIPKCNFDGSDCQPSFFSQNLSWIIVLIVIGILIILSIIFTIIYVMYQRKLEKERQNLLWQIKFSELEKPSEKDNLTKSTRSFQSGVSSTSTKITIDSKVDTEFHSFYIWNNENVVGRKSNVRIKLGDKECKEMRLLRALDHDNLCKLLGMSIDGINLIVIWRYCSRGSLYDVIEQQTTQMDDFFCYCLIKDVVSALDFIHDNPALAYHGHLTSKVCLIDERWQIKISGYGPKFLQSLETKSPTTNLWTAPEILREPSLIGSPTADIYSFAIIMSEVVNQKTAWNLDEIEENEDDIVYKVKRGGANLFRPKLVPDSRLQVNSSVLHLIKDCWSENPTDRPKTSTIKSLLKSIHSNKGENLMDHMFGIMEQYASNLEQEVEERMKELIEEKKKADILLYRMLPKTVADKLKLGQTVQPESFESVTIFFSDVVSFTTLASKSTPLQVVTLLNELYTTFDAIIDENGVFKVETIGDGYLCVSGLPVRNGNEHAKHIADMSFGFLRSLKTFRIPHIKDGKINIRIGIHTGPVVAGVVGLTMPRYCLFGDSVNIASRMESNSKPGRIQISTETNRYLTDIIGGYRTEPRGEVIVKGQGVMQTYWLLTGEETPEDLEEMRQQ*</t>
   </si>
   <si>
-    <t>MLLQILPLTVLFYLTTGQQKNTTLPATLLNTTKIMKNFNIPPYSKRPPFPFNESITINIGFLIPKDDVEFEDTVGYHKTASAIMIGLNELIHAGFIDTTKINFKFFFRFSNCSVLQGTKTTIELLQNDNVDVFFSVACQELSDFVSVIAASYGTPLYLWGPTVSTYIVDSNQLRSVISTSISTEDYSNSIRCLVDYFNWTKIAIVYMTTSTHPVCGYIQSNLVNTVLTTTKTVVVYSGQINTSTSSIVENLSAISKVARIVIVCIPLNEWKRKFMLTAYDLGMANEEYVYLLMDLNDTVIENIAETIPLWKNSNELEDKRDNDALEAFKFTLLIDKTAENNVDMEKFAKNISQGMLDYPFYCNETACLKNANDPNFHYSTYAPYLADTMILFGLALNRTLSTTPLLYTDQYTLKNNSAYSFDGFSGNVVLDNNTVRYGYFFVKYIGNDSKIYTNMIITKNENKTYYVNEYETSTENEIWWNRKNSARPLDTPICSFLGYRIRQQHQLDMLWLINYTELKSIKIQERIYGKSIASINESQRTLNKDIENSTHKNNNNGLCLNEKENRRHIAYRYNDETVVGERFPGSVIITTIERNHLRMLRNIDYECLNKFLGLAETPTYVIVVWKFCVRGNLKDLLKSKIGEIDPYFVVALMNDISNGIQYLHSSKINCHGRLTSSCCLLDSNYQIKLSNFGLPFLRKFVKRSYEEQLYTAPELLRNQNLLGTKEGDIYSFAIISSELLNKSLEWPEDEISHTKTDIIMKIKNSRRGTFRPIISYEIKERWVGEVINIIKDCWNEDPLKRKKIEIVIKMIKKSMNNKKISMMDYMFNKMENYASHLEAEVMGRTKELMEEKKKSDILLYRMIPKSVADELKSGRTVAPEYFESATVFFSDVVNFTNLCAQCTPLQVVNFLNQLYSQFDEIIEKFDAYKVETIGDAYLVVSGIPIRNGNKHGEMIANMSLEFMKTLPLFKLSFLPDYKLNLRIGLHTGPVVAGVVGLQMPRYCLFGDTVNTASRMESNGMPGCIHISSEMYELLSQFDNFKIECRGEVMIKGKGLLITYWLLGNINNNFEIKINDSNTVNSNDK*</t>
-  </si>
-  <si>
     <t>MYLKFILLLICIKLTFCLRTIKVGFLFPLQSSTLYNISGFNLSAGAVPIVFDKIREEQILPNFNFSFDVRFDECNLAKVVGQSDELIKNNIDVVIGPTCSLAATKSSLHLTFYNKPTFTWGISANNAYMDTKRLPNLITINPLISPIIIALIDILKTFNWWNIGLISTTNELGRCSNIRKGIENAIQTDVSHLSVKVSYETNIPPNENDYDMFLNDVKMNARIIIGCFDSDYWRRKFFLKMFDHQMNNNEYVFINFENRNSNFMQFEIDKTATRRLLIYEDYNTPNDGRDEDAYQIAQYTLYIDLATSSQIDFEFNKNVLNRIKEWPFYCETCNTSSAKLPSIFASYLYDSIYLWAKILNKTYNIYGEKALTDGSLYRKYCKGTYNGITEKFTYDDNCFRIANVELTGLSGKYNTTTYIKYKFSNISTFIKQNLVDDLKTTLFKKWGNKIPLNIPKCGYLNNKCFENFIENNKVLFIIICVIIFIIVIILFLIIIRIIFIIKKRKTNELLKWKILFSHLERYEEKNSLAKSMTSFQSGITSNSSHIKFKNYKESTKYLYAFYNDQLVVGEKHSFNILNIKEIQKELNDILLFEHKNINKFFGMCIEIGKIISIWKYSERGSLFDFLQTDSSIFDTFFCNNMLTDLLDGLNYIHNSSINFHGLLTSKKCLISSHWQLKISSFNCKSIRIKDKISSIDKLWMSPEMLRSEEYIGSQESDIYSLGIIASEVFTKSSPWNYCNRKESIDEIIYLVKNNSENTFRPELHIAKGLDISPKALDLCQECWKENPNDRPKLNNLITLHKHFNISKAKNLMDHVFFTLEDYAQKLKNEVNERCNEIQEEQKKSDILLKKMLPPQVSEKLKLGISVPPEDYNNVTIFFSDIVKFTNLSHKCSPFQVVNILNELFSQFDNVIESLDIYKVETTGDGYLCVSGLPNRNENNHVVEIAKLSLAFIEICNNFKISHLPNEKIMLRIGCNTGPCTAGVVGLSMPRYCLFGDTVNTASRMESNGKPGRIHTTESFYRLLSTFGNFIMEHRGEIIIKGKGVMNTYWLNDTT*</t>
   </si>
   <si>
     <t>MTHSIESSTPNFPPIDIVIALPKDGTNKKTNPYGLDMLKSKPVFDVVLEDIYYEKKLLPVNFFRLTYVDTENSDAIGPQRVIDRYCANKVDAVMGLPYVYGLAPIARFSVFWNLGVPVFSTSAKVDIFSNREQFPLLTRLTESNARLGSVFDQVIPIQAKKLFFYFHEQENQTLGIGKSECYFTLKAMKNNIRSDKFGEDHSSRTFNEHTNDKKSLFHQHIKNLKAASFISKVIILCASPDTVRDIMLAAYDLGMTQSGEYVFINIDVSTGSHAEQPWLRSNDTNPKNNEIAEQAYKALKTISLRRSAMAEYDDFEKKVKKRAEEVYNYKNITGKEYEMNNFISAFYDAVLLYAIALNKTISEGKDARSGKHITNKMWGITFKGITGNVSIDKNGDRYSDYSLLDLDPKERKFVEVAYYSGNKNELKKVSDFHWVGGSPPKDSPVCGWDNSLCNNGEKYYPHLLVAAIVVIIFLAAAFIFFYRRYRLEKEIAAMSWKIRWEELKSKNSESHEKKYFKKKHKSHKAVLYNDPNADQHDALLRINSNGSVNSDKFTDEDPEYMNMRQRLRSSSSGATRKISAMIFDRKLSLFTRKKSSPTSDKVLDLHNGNYDENNTSSPIDTGNKKLGTHSEDLEYGNGGFSFKNRKLSVQYSNGSVKSGGSVETIHMASNSKIFIRYAYYKGQTAAVKMLKIDPVKYPKLELSRDTLMEFKRIREYSHDHIIRVMGACVDPPNYCIVTEYCQRGSLEDILEDEKIKLDTMMKFSLLHDLVKGMNFLHHSEIRSHGRLKPSNCVVDSRFVLKITDYGLNELRAYEEISQEKDDSHEYWKKFMYTAPELLRLPNPPRGGTQKGDVYSFGLITHEVVYRCGPFYRGDESPDPKFIYEQIFKGPSIGKEVYRPILLDEVPNDEGGPSKPENMEQLTALMQRCWSENPMDRPEFSEIRKIAGSLNKDNETTNLVDNLLKRMEQYANNLETLVEERTQEYLAEKKKVEELLHQLLPPSVAVQLIAGNSVQAESYDCVTIYFSDIVGFTSLSSVSTPMQVVTLLNDLYLAFDGVVDNFKVYKVETIGDAYMVVSGLPERRDDHASQIAQMSLALLHKVKTFVIRHRPKEQLKLRIGMHSGSVVAGVVGSKMPRYCLFGDTVNTSSRMESNGMPLKIHVSSQTYDILSKDPDFHLELRGEVEMKGKGLQTTYWLKGYKDQQIPDFGPDYSNYKMPLKKQ*</t>
   </si>
   <si>
-    <t>MVNNKKLYGIIDEKDNNLKIRKQRNTNNNNSTLPFDKKVITISYLSALSVFPKNLYDYIKTVTNSSNTSNLFKNKSDKLDISSSYNFVSKCFRADFDGSVISGALKFAVDEINSNPNLLPNYHIQYVFNNTCGDETLSTKYFMDHWKSGVSAFIGPEMNCRTEAQMAAAQNLPIIAYKCKDEAVSNKIKYPTFARTVPAESAIAKTVIATLKEMNWKKVAIIYEEATSYSKLVDSIKVTMEQQNRHLKVNNKFEILSINTVPSPFSEFNDNKFDQIVGDTKDFSRIYLVVGTPKMGRKLTKVMGDKNILSSGLYLILLVCPDYDWLNLYHAMNNHFFRDTSEWLSKSWDVYNSDDHKFLKYAQYLLAIIPTPVSLNNPQVKYFWKKCNENLKYFGIHSNPFEKEIKPNRHAYYLYDAVMLYAKSLHQVINYYNKNGLNSDLAIKDGQMIMSYIIGKRYFSIQGFEMKINKNGNAIGNYSLISLQKVEPIYDKNNPNYYPIKYALNVTADFIDVDDGLLTLPKMRYHKNILWPRSSPPLDEPICGFMNDKCSYLSFKHYFEKKLRLEEIPDTWKIDIKKIEKISKNSETFKSLLFFDEDGGIFSDEFTKILARYIPKSTFKKNNLLDCGNQKFLKLSGIGLYEGTFVVIKEFTYDHDRKIISDLLKKECNIMKQLRNDNINNFIGLLIGPYSIYAVREFCGRCSLMDIYKNNDFKLDNLFISSFIDDLIKGMLYLQNTDVKIHGNLKSTNCLITNRFVLQLSDFGLYELRYGQNFKTEELMWEGLLWTAPELINFDDVAKPKPGTQEGDVYSFGIILHELVTGDGPFRLLSKNNICAAEIIKSIVEDDNFRPDTKFLNCPKFVIKCMKECWQKCPKSRPTFQNGIRQYLLPMLEQVMKNNLMDNMMALMDVYQNQLEDLVERRTLQLQNEKRKSEALLQRMLPPSVANQLIKDGKVRPEFYESVTIYFSDIVGFTDLANFSTPIEIVSFLNDLYTMFDSIIKKYEVYKVETIGDAYMVVAGCPKYYSASKQAEEIASMALHILACSSTFVIKHKKNEKLSIRIGIHSGCVAAGVVGKTMPRYCLFGDTVNTASRMESTGSGMKIHCSIDTRSLLESKENFLFEHRGFQYIKGKKPVLTYWLLGRTDWNENDNCYNDLKNNKLRNSKLFFTKNDKKYKIYNKSLNKLKYFKNRSKNNYECNCLNEEYEEYDINESFKIPNSLNELSLFEYKKNSLNIIKDKEKYIFQKSLSFPLLNKEKLYKWDNENAMSFKKLSRECSIMSSTSNLESTFSENDYNNDESKSIISKNDSLDDDSDYSYETSGSKSSSISSFNAYKRLPHFNKYILKDSYDEEVLKNKIYKNDNIIKRVKCMNYDNYKKISRYFRNPTLMEYKLLSKNSSSDEGYMDRYAVNKSKFNDCNEYDLEAAKSWNNSTIKNSYFPVNRNRNLSIIKNNETNTDNDESISYEESLITKTPSFFNQRKDIRKNQKSNLFINEDYGGLTDQ*</t>
-  </si>
-  <si>
     <t>DGFFIYSLIKDIVEGLYVMHNSAIEYHGNLSSKNCLVDERWQVKLSDYGFPFLRCLEEPKSAREQLWTAPELLRNKELRPNQSSDIYSLSIVMADLVNKNISFENSDVQKEADEIIYLLKNRNSESTRPTLNPAVENINGNLLHLIRDMWAEDPSRRPKISVIRKLINDMNETKSKNLMDHMYDLLENYAASLEEDIQHRTKELMEEKKKADLLLSRMLPKAVAEKLKLGQPIAPEHFDSVTIFFSDVVSFTTLA</t>
   </si>
   <si>
@@ -537,9 +488,6 @@
     <t>MKKLFNFKFIIFFLFFFISLYHFICGRKSILNTTNIIKSFEIPSYQNTQPFPYKNLTIKIGILIPEDNNETSDSIGYYKTASGVTIGYYDLLNAGFIDEKKLKFDFFFNQINCTKLDGTKNAIELLIINKVDVIICPPCKNLANFISVIYTTYNRPVYLWGTTINSFLSTSNEIQTVISTSISVIDYTYTMIQILQHFQWKYVAYVYMVIPSDNKCLQMQNDFVTNVLKNTDIIVGYVGELNTSTTSMKEILNEIKKQARIVIVCIPTIIYNRKFMLTVYDEGMANNDYLYILLGVDDSIFQNYINYTSLSEVKQISNYDRNEDFMEVIKYTLILNKETKGQNIQTNIFSNEIKNYMIEWPVNCNDTICLKNVNDPNFQSSIYAPHLADTMILYGLALNKTLSTEPLKYNDGMLIKNNSLSEFDGYTGTVDFGNDGIRLGYFYLFTYNNNSDTVNLLKIYEINKEQYIVKKLYKNEEEIWFNRLDKKRPIDKPICGFENNECETSNFNIYVKYIIIIIIIFAILIIGTIILIIYIKKSKIKQQKLLDKIWLIKYEDLEIINLRKIYSSRTVSSSKSIETSLNTFKLKNENDVKIAYNEDYIEDDNVKFIGYKYKEDIVIGEKFHKYFNIDNKIRSHLRFLREIDHENINKFIGLTEYRKYLIPIWGYCSRKSLKDWIINNKNDLEPFYIISLINGIASGILFIHTSKIGYHGRLTSSKCLLDDYFQVKITSFGLKFISEQYQRTENEQLYTAPELLRTLSLTGTKEGDIYSFAIISSELLNKSPAWFNKHEGMLIQEIILKIKNSKLGNFRPIIEDNYNEEWIKDVIKLIKDCWDEDPLRRRKIKTIKKMLKNAVKVKNINLMDYMFKKVENYAAELEEDVKIRTRQLYEEKKKCDQLLYRMMPKSVVEKLKAGENVQPEYFKSATVFFSDVVNFTNLCSQCTPLQVVNFLNQLYSQFDEIIEKFDAYKVETIGDAYLVVSGIPIRNGDNHGKMIANMALGFMNALPSFKLSFLPDYRLNLRIGLHTGPVVAGVVGLQMPRYCLFGDTVNTASRMESNGMPGCIHISESTEELLSLTGEFRITKRGNIIIKGKGNMFTYWLLGKENEPEKWLKEPE*</t>
   </si>
   <si>
-    <t>MCYKELLEDKVFDNTFDIQFVFSRSCGKNYEGVGVAVEMYHIQNVKCFIGPYCNSEMEAVSKMSAYWNIPVIGYIASSNIFSNKNIYKTLARVTRKTNNNLAITVSAMLKYVGWKKVLVVIGDEQIAYERLTSFEEHFQENNITISRKVTLDENLNSNEIIKSGIINEIKSYGRIIVCIFSKTSQISQVFMEAISQSNTKTNDFVYIFPWLQTDVKERLPWIGKNGEVNQIVKKSFDNTIIIDDIFSFNDTVVEHFKQKMSKNNIDINQLDLNNIYGYIQLYDSLKLYALVVKKLIKQSNGDFNVTNNGKLIWDKMRRFSFPGFMYNIGLVSENLIMDDLAEQMASYGAFFISPKQDDILNVFEIEPVLKENCDSFKTKSGCFEMKIISVVKNFWPSIDGELPLDEPTCGYKNEKCNYTIYIVTGCVIIFLIVLIIVIFIVSRILENKALEKTPWRVWRDDLRIISEEEMESVVSMESFKTRISNINKLIKYHAILGTNTHTSFHLYPQKSYIQFSREDIILLTEMKKLVHDNINPFIGISFNEKDEMLILWKFCSRGTIQDIIYNDNVVLDDKFHAAFIRDITNGLEYLHFSTVRYHGSLTPWCCLIDRNWVVKLTDYCIANPIEKWTRKKLIDPESIRLGDDKSAATQKTNVLYCAPEVLKTSKENQRRRIDQSWIKQSQAKRQAGDIYAFGILMYEILFRKLPFNEDVCSSELVDIIKSDTNDIKPVIHDYSKLHSDLVALLLDCWHPNPDIRPTIRRVRLNTENCLKVKGSIVDQMMRVMEQYANNLEKLVHERTAMLEEANLKADNLLAQLLPKYVANELKMGRSVPPRIFQETSVMFSDIVEFTKLCSNSTPLQVVNFLNSVYAGFDDIIKQYDAYKVETIGDAYMVVSGLPEENGKRHLAHLSNIALDIILFLNEYVIPHRKNQELQVRLGIHCGPTAAGVVGLTAPRYCLFGDTVNTASRMESTGVRKQIQVTEVFKESLSLHYPEFDLSLRGFTEVKGKGSLVTYWLIGRNGQQITTSLNQNT*</t>
-  </si>
-  <si>
     <t>MVSIIILLIILTTKVFPKSVGILKVGLIFPNIEPVLIKYMGYQNSASAVVIAFKEAKKEYPILKNLTIEIVCDYTECLSFEVSGKAYDLIKKNKINVLIGPPCKKTMEIVSSIATYYNIVTLFWGNTFTYLPNKYNDKNIVGNIMGTYSDMNHCLANILLKFDWVSISLIYQSTYYELEMCEKYSESFQNILTTYYEDILIVYRKKIVSTKKEDLKEIADDIKKVSRIIIMCFSEREKEEKMLLQFYDNNMNNQDYVYINIDCSMVAYEDSKNQKLINTLDVHLNNNDKKLLSMYKWIYNFKFSLNGMRGHLYSDVKKSVPKLMKESPFYCIEECSEYNTSSHYAPYLFDAAYIYFLTIGNLLSSQKVANFSNISYKNIIKKIPGHYNGATGLYRINKNLTRDTEVTFSRYDYYNNSIIHLIKGSRTENATIITYLYTDPKTTIWYYRNGEQPLNVPKCGYSEELCQPTFIESSPIGFAGIILGSIIIILIIIGSIIYGFYTKFKQEKLDNLIWKIDTLDITNYSNYIAKKNEGQSKISLLSSICSNGKTNFQSLEERKHILYIYKRKIIVGTKHEVHYTLNKKDTIELRNLKMLNDNHLNQFIGFYNSPSYSISFWRYCPRLSLVDVFQLESLKSKIDNFFIYSFISDAIDGMEIIHKSPIKVHGNLMLNNCLVDERWKLKLSDFGMRFIREREKRDKKDLLWTAPELLKEEILQPNQNSDIYSLAIVMVDIINNNISYCNSKNEIEIDEVIYMLKNKKNEFFRPEISPVVDNIPNTMFHLIEEMWAQDPNTRPSIGVVNKLIKSMNPSKSNNLMDHIFNILEDNAITLEEEINLRTNELIKEKTKADLLLSRMLPKQVVEKLKSGQLIQPEYFDSVTVFFSDIVSFTVIASKCTPLQTVDLLNNLYTLFDSTISKHDVYKVETIGDGYMCVSGLPIKNGDLHVKEIACLSIDLVKKMPEFDVSYLPKGTVKVRIGIHSGSCIAGVVGLTMPKYCLFGDTVNIGSKIESTGKANQIHMSDKAHLLLTQKIGGFVTESQGEIIVKGAGVMNTYWLLGTEDEIIYTPIK*</t>
   </si>
   <si>
@@ -690,9 +638,6 @@
     <t>SRAE_2000417200.1 split 1</t>
   </si>
   <si>
-    <t>New split blastp pulls up: gcy-13, gcy-20, gcy-14, gcy-22, etc. The original on WBPS had two protein kinase domains associated with it. I think it's two separate genes.</t>
-  </si>
-  <si>
     <t>Reverse blastp yields strong match to gcy-35 - this is probably a soluble GC</t>
   </si>
   <si>
@@ -738,12 +683,6 @@
     <t>Yes?</t>
   </si>
   <si>
-    <t>Didn't previously have a clear homolog in Rebecca's dendrogram, by tblastn matches strongly with SRAE_2000427200, alsto SRAE_2000427100 and others</t>
-  </si>
-  <si>
-    <t>Didn't previously have a clear homolog in Rebecca's dendrogram, by tblastn matches strongly with SRAE_200042700</t>
-  </si>
-  <si>
     <t>This has lots of zinc fingers in it, no cyclase domains. Seems unlikely to be a real hit. This "matches" to SRAE_1000175800, which had two genes in it that needed to be split - I'm betting the bit it matches is the bit with the zinc finger region.</t>
   </si>
   <si>
@@ -765,9 +704,6 @@
     <t>Blastp matches to Ce let-418, chd-3, tblastn matches SSTP_0001276200, as predicted</t>
   </si>
   <si>
-    <t>No evidence in the RNAseq for this?</t>
-  </si>
-  <si>
     <t>SRAE_0000025200.1 split 1</t>
   </si>
   <si>
@@ -792,21 +728,9 @@
     <t>Match is only 29 bp/AA; protein has cadherin-like domains, no nucleotide cyclase domains</t>
   </si>
   <si>
-    <t>Based on tree, matches closely to 2 SSTPs</t>
-  </si>
-  <si>
-    <t>Dendrogram: also matches to SRAE_2000494300 - looking at the Sr and Ss genomes, the genes flanking this one and SSTP_0000937800 are a 7M GPCR on the 5' forward strand, and a protein with an alpha/beta hydrolase on the 3' reverse strand. those same genes are flanking SRAE_2000494300.</t>
-  </si>
-  <si>
-    <t>Ostensibly matches SRAE_2000427000, which is 1076 aa, with 7 exons, lots of small introns. I tried to shift around the exon to get a longer ORF for exon 2, although given the RNAseq data I'm not convinced this is accurate. However, the new protein is longer, and matched via Blastp to Ce-gcy-5, 7, 17, 14, etc... tblastn of protein back to S. ratti genome got me ,matches to SRAE_2000494300 (as does SSTP_0000937900. Looking at the Sr and Ss genomes, the genes flanking this one and SSTP_0000937900 are a 7M GPCR on the 5' forward strand, and a protein with an alpha/beta hydrolase on the 3' reverse strand. those same genes are flanking SRAE_2000494300).</t>
-  </si>
-  <si>
     <t>STP_0000354100</t>
   </si>
   <si>
-    <t>Seems to really not have a direct homolog, in the current genome.</t>
-  </si>
-  <si>
     <t>Has a GC domain. But the majority of this gene is missing b/c it's on a contig that cuts off at the 5' end of the gene. tblastn to Sr yields: 	SRAE_2000427000, SRAE_2000427100, SRAE_2000427200, 	SRAE_0000025200; tblastn to Ss =&gt;SSTP_0000962200, SSTP_0000962300, SSTP_0000962400</t>
   </si>
   <si>
@@ -816,13 +740,157 @@
     <t>This is too short b/c the contig cuts off at the 3' end - doesn't have a protein kinase domain or a transmembrane domain</t>
   </si>
   <si>
-    <t>Yes-ish</t>
-  </si>
-  <si>
     <t>Contig cuts off at the 3' end, but does include the transmembrane domain and the protein kinase domain. tblastn to Ss-&gt; SSTP_0000962300, SSTP_0000962400. tblastnto Sr-&gt; SRAE_2000427000, SRAE_2000427200, SRAE_2000427100</t>
   </si>
   <si>
-    <t>Eh?</t>
+    <t>MLLKILSLILLFNLITGQQTNTTLAANLLNTTKVMKSFNIPSYSERTPFPFNGSINVNVGFLISKGDADYEDTVGYYKTASAIMIGLEELIHAGFIDTTKVQFKFYFRFSNCSVLQGTKTTIELLQNDNVDVFFAVACQELSDFISVISTSYGTPLYLWGPPISTYIVNSNEKRSVISTSISIEDYSNSVKSLVDYFEWKKISIIYMTTTLHSVCGNMQTNLINTVLTTTKTVVVYSGSVNSSGDSMVENLLAISNVSRIVIVCIPSNDLKRKFMLTAYDMGMTNDEYVYLIIDVNDTVIENSDDSIPVWKDSSNLQDDRDEDALEAFKFALLIDKTAENNVDMKRFARNISKGMLDYPFYCNETECLKNSKDPNFHYSTYAPYLADTMILFGLALNRTLSTTPLLYTDKDILKNNSAYSFEGFSGNVVLDNNTVRYGYFFVRYIGNDSKIYTNMIITRNKNQTYYVHSYGTSNENKMWWNRKDFSRPLDTPLCSFAGNKCPKTFWEEYFIIIIIVIITFIGILIFSIIVIILLRRYRIRQQRQLDMLWLINYEDLKSIKSNERMYGKSVISINDSQKTLNKDIEILNNKDNELNLNERDNRRHIVYRYNDETVVGEKFPKSITITSAERNHLRMLRNIDHECLNKFVGLTESPTHVIGVWKFCVRGNLKDLLKNKVREIDPYFVVALMNDISSGIQYIHSSKINCHGRLTSSCCLLDSNYQIKLSDFGLSFLRKYIKRNFEEQLYTSPELLRSQNVLGTKEGDIYSFAIISSELLNKSLEWPEDEISHTKNDIITKIKNSRRGTFRPIISYEVKERWVGKVINIIKDCWDEDPLKRKKIELVRKMIKSSMNNKKISMMDYMFNKMENYASHLESEVMGRTKELMEEKKKSDILLYRMIPKSIADELKSGRTVAPEYFESATVFFSDVVSFTNLCAQSTPLQVVSFLNQLYSQFDEIIERFDAYKVETIGDAYLVVSGIPIRNGNKHGEMIANMALEFMKALPLFKLSYFPDYRLNLRIGLHTGPVVAGVVGLQMPRYCLFGDTVNTASRMESNGMPGCIHISSEMCELLTQFDTFEIENRGEVMIKGKGILNTYWLLGNINDDFKLKVNNSNTVNTNDK*</t>
+  </si>
+  <si>
+    <t>MLLQILPLTVLFYLTTGQQKNTTLPATLLNTTKIMKNFNIPPYSKRPPFPFNESITINIGFLIPKDDVEFEDTVGYHKTASAIMIGLNELIHAGFIDTTKINFKFFFRFSNCSVLQGTKTTIELLQNDNVDVFFSVACQELSDFVSVIAASYGTPLYLWGPTVSTYIVDSNQLRSVISTSISTEDYSNSIRCLVDYFNWTKIAIVYMTTSTHPVCGYIQSNLVNTVLTTTKTVVVYSGQINTSTSSIVENLSAISKVARIVIVCIPLNEWKRKFMLTAYDLGMANEEYVYLLMDLNDTVIENIAETIPLWKNSNELEDKRDNDALEAFKFTLLIDKTAENNVDMEKFAKNISQGMLDYPFYCNETACLKNANDPNFHYSTYAPYLADTMILFGLALNRTLSTTPLLYTDQYTLKNNSAYSFDGFSGNVVLDNNTVRYGYFFVKYIGNDSKIYTNMIITKNENKTYYVNEYETSTENEIWWNRKNSARPLDTPICSFLGNKCPKTFWEEYYIIIIIVVITFISIFIFTIIVIILFQGYRIRQQHQLDMLWLINYTELKSIKIQERIYGKSIASINESQRTLNKDIENSTHKNNNNGLCLNEKENRRHIAYRYNDETVVGERFPGSVIITTIERNHLRMLRNIDYECLNKFLGLAETPTYVIVVWKFCVRGNLKDLLKSKIGEIDPYFVVALMNDISNGIQYLHSSKINCHGRLTSSCCLLDSNYQIKLSNFGLPFLRKFVKRSYEEQLYTAPELLRNQNLLGTKEGDIYSFAIISSELLNKSLEWPEDEISHTKTDIIMKIKNSRRGTFRPIISYEIKERWVGEVINIIKDCWNEDPLKRKKIEIVIKMIKKSMNNKKISMMDYMFNKMENYASHLEAEVMGRTKELMEEKKKSDILLYRMIPKSVADELKSGRTVAPEYFESATVFFSDVVNFTNLCAQCTPLQVVNFLNQLYSQFDEIIEKFDAYKVETIGDAYLVVSGIPIRNGNKHGEMIANMSLEFMKTLPLFKLSFLPDYKLNLRIGLHTGPVVAGVVGLQMPRYCLFGDTVNTASRMESNGMPGCIHISSEMYELLSQFDNFKIECRGEVMIKGKGLLITYWLLGNINNNFEIKINDSNTVNSNDK*</t>
+  </si>
+  <si>
+    <t>MVNNKKLYGIIDEKDNNLKIRKQRNTNNNNSTLPFDKKVITISYLSALSVFPKNLYDYIKTVTNSSNTSNLFKNKSDKLDISSSYNFVSKCFRADFDGSVISGALKFAVDEINSNPNLLPNYHIQYVFNNTCGDETLSTKYFMDHWKSGVSAFIGPEMNCRTEAQMAAAQNLPIIAYKCKDEAVSNKIKYPTFARTVPAESAIAKTVIATLKEMNWKKVAIIYEEATSYSKLVDSIKVTMEQQNRHLKVNNKFEILSINTVPSPFSEFNDNKFDQIVGDTKDFSRIYLVVGTPKMGRKLTKVMGDKNILSSGLYLILLVCPDYDWLNLYHAMNNHFFRDTSEWLSKSWDVYNSDDHKFLKYAQYLLAIIPTPVSLNNPQVKYFWKKCNENLKYFGIHSNPFEKEIKPNRHAYYLYDAVMLYAKSLHQVINYYNKNGLNSDLAIKDGQMIMSYIIGKRYFSIQGFEMKINKNGNAIGNYSLISLQKVEPIYDKNNPNYYPIKYALNVTADFIDVDDGLLTLPKMRYHKNILWPRSSPPLDEPICGFMNDKCPVNIFFKYIWAFIFFFFFCLLGSYLSFKHYFEKKLRLEEIPDTWKIDIKKIEKISKNSETFKSLLFFDEDGGIFSDEFTKILARYIPKSTFKKNNLLDCGNQKFLKLSGIGLYEGTFVVIKEFTYDHDRKIISDLLKKECNIMKQLRNDNINNFIGLLIGPYSIYAVREFCGRCSLMDIYKNNDFKLDNLFISSFIDDLIKGMLYLQNTDVKIHGNLKSTNCLITNRFVLQLSDFGLYELRYGQNFKTEELMWEGLLWTAPELINFDDVAKPKPGTQEGDVYSFGIILHELVTGDGPFRLLSKNNICAAEIIKSIVEDDNFRPDTKFLNCPKFVIKCMKECWQKCPKSRPTFQNGIRQYLLPMLEQVMKNNLMDNMMALMDVYQNQLEDLVERRTLQLQNEKRKSEALLQRMLPPSVANQLIKDGKVRPEFYESVTIYFSDIVGFTDLANFSTPIEIVSFLNDLYTMFDSIIKKYEVYKVETIGDAYMVVAGCPKYYSASKQAEEIASMALHILACSSTFVIKHKKNEKLSIRIGIHSGCVAAGVVGKTMPRYCLFGDTVNTASRMESTGSGMKIHCSIDTRSLLESKENFLFEHRGFQYIKGKKPVLTYWLLGRTDWNENDNCYNDLKNNKLRNSKLFFTKNDKKYSKNNKKILSLKHNNNIEIYNKSLNKLKYFKNRSKNNYECNCLNEEYEEYDINESFKIPNSLNELSLFEYKKNSLNIIKDKEKYIFQKSLSFPLLNKEKLYKWDNENAMSFKKLSRECSIMSSTSNLESTFSENDYNNDESKSIISKNDSLDDDSDYSYETSGSKSSSISSFNAYKRLPHFNKYILKDSYDEEVLKNKIYKNDNIIKRVKCMNYDNYKKISRYFRNPTLMEYKLLSKNSSSDEGYMDRYAVNKSKFNDCNEYDLEAAKSWNNSTIKNSYFPVNRNRNLSIIKNNETNTDNDESISYEESLITKTPSFFNQRKDIRKNQKSNLFINEDYGGLTDQ*</t>
+  </si>
+  <si>
+    <t>SSTP_0000214200.1 extended</t>
+  </si>
+  <si>
+    <t>SSTP_0000489700.1 extended</t>
+  </si>
+  <si>
+    <t>SSTP_0000937800.1 extended</t>
+  </si>
+  <si>
+    <t>Matches to SRAE_2000417200.1 splits - Is missing a transmembrane domain - at least originally? Realized there was an extra intron that removed the transmembrane domain. it's now there.</t>
+  </si>
+  <si>
+    <t>MKYLSLSMFYIFILVFNFVFIINGINVTFLRNDGNTTIACTTAIEHAKSSGQCQDDIYLKIGDACRIGNDALGTVAACDFFYNENAKAIVGPECFDESSHLALLSYHWKIPLFSPNGKVVYNYNNTVFPTVIHTSFSNVVLYANSLMLFMNRFNLSSVTFLGPKDDRNIHFRSIFEGVNKYFKTYFYNITTNIISIEESRLSSYNPKDIGLISFIKLIVIDTSFNDLHSVLQQMEVSSLYDHGYIFILLCSQHSSVCDSNIDKIILDCNMLLLGPYFKNYTDIDLLMSQYFKDSYNRFKGINYLSTYISCYSSCVASKLNTNLDGTSVVNTMKGKQLNTSLGNFIFDQMPSILITQSFSQYDSVNNTFVDLILTNPIASTCSKNKCFNLEIKVNNDEFWKSQLASPLTHCHLFKNCTNYLVIILCVTGAVVLIIILILIYMLRRQRRLNVYRMNWKIPKSQFKVIENKVSNSKKQGNTAETLSSKRRYIHAYAIVDTTKAEFLQLRQLKKIVWSKPEIKFITELKKISHDNLTNFLGVNYNDTDKFYMLSSLIDRASLEDLVDDTDFNLDMTFKSAFIRDILKGLQYLHKSFIGYHGLLNIQTCLIDANWVLKLSNFGITNILHNLIHDEVLKNIELINLHFYQTISPENLQGCNFGINYPMGSQNGDIYSFGIILYRLTYRHGPFDHVSMVPKDILKEIVKNTIEPTFDETLEDNSLLDLMKNCLKFNHLERPSLKVLESSITTILHSTRGNLVDQMINMNEKYAQNLEKVIAERTNMLVEAQLQTDRLLSEMLPRSIAETLKNGGTVEPKLYESATVCFVQICDFAKFMEENLPPAVMSFLNDIFNMFDDVIHNYDCYKVETIGDTYMVVSGVPKENEGKHVFVIAEVAISLRSHSLHYDVPVKPDWKLQVRIGFHCGPIAAGVIGLKAPRYCLFGDTVNFASRMESNCPANQIQVSESTALKLMENPEYRLIKRGIVKVKGKGDVNTYWLNEHFHQNEILSASKS*</t>
+  </si>
+  <si>
+    <t>MKYSLLSMFYIFIFIFNFVFIIRSTNVAFLRSDSNTSVACAIGIEHAMSAGQCQDNFFLLYGDACVVDSDALGTVKACGYFYNENAKVIVGPECYDETSHLSFLSYHWKIPLFSQSGKIWFGYNNTIYPTVIHTSFLNVVLYADSLMLFMNRFNLSSITFLGPKNEKDIHFKPLFEAVDRYFKVFYTNITTNIISIDESMLSYYNPRDIGLISFIKLIVIDTEFNDLNNVLQQMEIPTLYNHGYVFILLCSQYSSVCASKFNKFISDYSMLLLGPYFENYTNIDSLMRQYFRDSYNRLKGIEYLSAYISCYSSCVASKINTNLDGTSVANSMKGKQLNTLLGNYAFDQMPSILITQSFSQYNSQNNSFIDLILSKPISSNCKDNRCFSLDFIVNNDKFWQSQLASPLTHCHLFKNCTNYLVIILCVTGAVILIIILILIYMLRRQRRLNIYRMNWKIPKNQFKVIENKVSNSKNKQGNTTETLSSKRRFIHAYAIVDTTKAEFLQLRQLKKIVWSKPEIKFITELKKISHDNLTNFLGVNYNDTDKFYMLSTLVDRASLEDFVDDPDFTLDITFKSAFIRDILKGLQYLHKSYIGYHGLLNIQTCLIDANWVLKLSNFGITNILHNLIQDEVLKNIELINLHFYQTISPENLKGCNFGINYPMGSQNGDIYSFGIVLYRLTYRYGPFDNVSMVPKDILKGIVENTIEPVFDETLEDSSFLDLMKNCLKYNHLERPSLKTLESNIKTILHSTRGNLVDQMINMNEKYAQDLERVVAERTNMLVEAQQQTDRLLSEMLPPSIAETLKNSGTVEPKLYESATVCFVQICDFPKFMEENLPPAVMQFLNDVFNMFDEVIHNYDCYKVETIGDTYMVVSGVPKENEGKHVFVIAEVAISLRSHSLHFNVPVKPDWKLQVRIGFHCGPIAAGVIGIKAPRYCLFGDTVNFASRMESNCPPNQIQVSESTALKLMENPEYRLIKRGIVKVKGKGDVNTYWLNEHFHPTEDSSN*</t>
+  </si>
+  <si>
+    <t>1 transmembrane domain, matches to SRAE_1000137800.1, which is extended in 5' direction - increased length to better match RNAseq. This could be too long though</t>
+  </si>
+  <si>
+    <t>2 TMD?</t>
+  </si>
+  <si>
+    <t>2TMD, is this gene too long in the 3' region? But matches gcy-12, also long</t>
+  </si>
+  <si>
+    <t>2TMD</t>
+  </si>
+  <si>
+    <t>New split blastp pulls up: gcy-13, gcy-20, gcy-14, gcy-22, etc. The original on WBPS had two protein kinase domains associated with it. I think it's two separate genes. Now 1 TMD</t>
+  </si>
+  <si>
+    <t>SSTP_0000912800.1 extended</t>
+  </si>
+  <si>
+    <t>SRAE_1000137800.1 split</t>
+  </si>
+  <si>
+    <t>multiple TMD</t>
+  </si>
+  <si>
+    <t>1 TMD</t>
+  </si>
+  <si>
+    <t>at least 1 TMD</t>
+  </si>
+  <si>
+    <t>MIDNKIFSFFIFIFYFKLLYSSSTTEIPIVLSTIINDNKTTNVTNNDLNKSENMSNVLSGSTIRKGKGKIVRIGHIGALNAMPNAELVLDMARKELWRDGILDDEFDVELINTRACGESFEGVAVAADMFHLQDVKAFIGPYCNAEMDAVSKMAAYWNVPIIGYMAASNTFSDKTIYKTLARVSIRTTNSLAYAVATTLKHYNWKNVAIVTNTGVVALERTVSFEENFHKLGINILRKITFDENADTKLILESGLMQDIKNTARIIICIFTKTRDMTIEFMKAVVQAKMNTNDYVYIFPWLQAEAKEPPPWIDKEGHINTNIKKIFSNSIIVDDINGFDNTLTTPFVEKMEKNNLDINELDLSNVYGYIHLYDSLKLYSLIVRSIMNKTGGDFDPLTNGKKIWNEMRRFSFPGLVSIEGTSAGNVIMDDLAERAASYGAFYINPDRDDVIKMVEMEPVFVNNCDGLKTKSGCYELKVSDIVTGFWPSPDGKLPFDIPNCGFKNEKCDYTLYIVIGVLSLLIIIFIILGLSISRILENRALANTPWRIWRDDTRTITEDEMKSMLSIGSSKTKISNMSKFVKHHAVIGTNTHASYHIYPQKRLITFAREDIKLLNQMKLLVHDNLNPFLGMSFNEKDEMLLYWKFCSRGTVQDIIYNDDINIDSNFHAAFIRDITAGLEYIHLSPVIFHGSLTPWACLIDRNWTVKLTDYTIASLVEKWTKLSMIDPEAIKDGENKAAATQKSYVLYCSPETLKTSETNKRKNNESDWVKQSGSRKQASDIYSFGIVMYEILYRSLPFSDTLNVDELIDGNKLGNANIKPSIQDRSKIHPDLCALLLDCWNINPEVRPSIKRVRLNTEHYLKVKGSLVDQMMRVMEQYANNLEKLVQERTGMLEEANIRADKLLSQLLPSYIANELKMGKSVPPKLFEQASVMFSDIVGFTKICSSSSPLEVVNFLNSVYTGFDDIINKHDAYKVETIGDAYMVVSGIPQENGVNHLANLADVTLCMMEFLQTYIIPHKKNEKLRIRLGIHCGPVAAGVVGLTAPRYCLFGDTVNTASRMESTGLPEQIQISTFFNDRLNKHFPEFDTSLRGPVLVKGKGEINTYWLEGKNGRSITAPIPVELQNQFGKI*</t>
+  </si>
+  <si>
+    <t>SRAE_2000430600.1 extended</t>
+  </si>
+  <si>
+    <t>missing a TMD, likely issue with introns. Used sequencing I did when isolating the cDNA for this gene in 2016, I confirmed that the intron between exons 3 and 4 in WBPS isn't real. When I generate a new exon that removes the spurious intron, the sequence has a TMD. This leaves the sequence with 4 exons, which matches the S. stercoralis homolog, SSTP_0000354300. the lengths now match as well.</t>
+  </si>
+  <si>
+    <t>1-2 TMD, 2 exons</t>
+  </si>
+  <si>
+    <t>MVNFYFIIIIFYIVINCQKIVTSSTEEPFFSTTITESVEINTNESSTSSNGLFVNKNKSSKNNQNIIKIGHIGAEDQLPLAESILEMCYKELLEDKVFDNTFDIQFVFSRSCGKNYEGVGVAVEMYHIQNVKCFIGPYCNSEMEAVSKMSAYWNIPVIGYIASSNIFSNKNIYKTLARVTRKTNNNLAITVSAMLKYVGWKKVLVVIGDEQIAYERLTSFEEHFQENNITISRKVTLDENLNSNEIIKSGIINEIKSYGRIIVCIFSKTSQISQVFMEAISQSNTKTNDFVYIFPWLQTDVKERLPWIGKNGEVNQIVKKSFDNTIIIDDIFSFNDTVVEHFKQKMSKNNIDINQLDLNNIYGYIQLYDSLKLYALVVKKLIKQSNGDFNVTNNGKLIWDKMRRFSFPGFMYNIGLVSENLIMDDLAEQMASYGAFFISPKQDDILNVFEIEPVLKENCDSFKTKSGCFEMKIISVVKNFWPSIDGELPLDEPTCGYKNEKCNYTIYIVTGCVIIFLIVLIIVIFIVSRILENKALEKTPWRVWRDDLRIISEEEMESVVSMESFKTRISNINKLIKYHAILGTNTHTSFHLYPQKSYIQFSREDIILLTEMKKLVHDNINPFIGISFNEKDEMLILWKFCSRGTIQDIIYNDNVVLDDKFHAAFIRDITNGLEYLHFSTVRYHGSLTPWCCLIDRNWVVKLTDYCIANPIEKWTRKKLIDPESIRLGDDKSAATQKTNVLYCAPEVLKTSKENQRRRIDQSWIKQSQAKRQAGDIYAFGILMYEILFRKLPFNEDVCSSELVDIIKSDTNDIKPVIHDYSKLHSDLVALLLDCWHPNPDIRPTIRRVRLNTENCLKVKGSIVDQMMRVMEQYANNLEKLVHERTAMLEEANLKADNLLAQLLPKYVANELKMGRSVPPRIFQETSVMFSDIVEFTKLCSNSTPLQVVNFLNSVYAGFDDIIKQYDAYKVETIGDAYMVVSGLPEENGKRHLAHLSNIALDIILFLNEYVIPHRKNQELQVRLGIHCGPTAAGVVGLTAPRYCLFGDTVNTASRMESTGVRKQIQVTEVFKESLSLHYPEFDLSLRGFTEVKGKGSLVTYWLIGRNGQQITTSLNQNT*</t>
+  </si>
+  <si>
+    <t>SSTP_0000846800.1 extended</t>
+  </si>
+  <si>
+    <t>at least 1 TMD, 2 exons. WBPS is cutting off the first part of the gene. When I add the earlier ATG on, the length better matches with it's ostensible Sr homolog. It also matches the version of the gene I have, so at some point the annotation was correct in WBPS and then got altered.</t>
+  </si>
+  <si>
+    <t>Alignment is very suspicious, as are RNAseq tracks (hits in introns); matches to SSTP_0000912800.1, is extended in 5' direction - this might actually be too long? Made shorter to match SSTP.</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>3 TMD?, 2 exons</t>
+  </si>
+  <si>
+    <t>1-3 TMD, 2 exons</t>
+  </si>
+  <si>
+    <t>Seems to really not have a direct homolog, in the current genome. 1-3 TMD, 2 exons</t>
+  </si>
+  <si>
+    <t>1 TMD, 3 exons</t>
+  </si>
+  <si>
+    <t>Based on tree, matches closely to 2 SSTPs, 1-2 TMD, 2 exons</t>
+  </si>
+  <si>
+    <t>2 TMD? 6 exons?!</t>
+  </si>
+  <si>
+    <t>2 TMD, 1 exon</t>
+  </si>
+  <si>
+    <t>2 TMD? 6 exons</t>
+  </si>
+  <si>
+    <t>2 TMD, 3 exons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 exons, TMD present. </t>
+  </si>
+  <si>
+    <t>9 exons, multiple possible TMD, There are RNAseq hits upstream that aren't associated with a specific gene, however this one has all the domains it should have. Also the levels of the RNAseq don't match the levels for this gene.</t>
+  </si>
+  <si>
+    <t>5 exons, all domains present</t>
+  </si>
+  <si>
+    <t>7 exons, all domains present. Didn't previously have a clear homolog in Rebecca's dendrogram, by tblastn matches strongly with SRAE_2000427200, alsto SRAE_2000427100 and others</t>
+  </si>
+  <si>
+    <t>7 exons, all domains present. Didn't previously have a clear homolog in Rebecca's dendrogram, by tblastn matches strongly with SRAE_200042700</t>
+  </si>
+  <si>
+    <t>2 exons, all domains present</t>
+  </si>
+  <si>
+    <t>6 exons, all domains present</t>
+  </si>
+  <si>
+    <t>1 exons, all domains present</t>
+  </si>
+  <si>
+    <t>2 exons, all domains present. Dendrogram: also matches to SRAE_2000494300 - looking at the Sr and Ss genomes, the genes flanking this one and SSTP_0000937800 are a 7M GPCR on the 5' forward strand, and a protein with an alpha/beta hydrolase on the 3' reverse strand. those same genes are flanking SRAE_2000494300.</t>
+  </si>
+  <si>
+    <t>6 exons, TMD and catalytic domains present</t>
+  </si>
+  <si>
+    <t>3 exons, necessary domains present. Near edge of contig</t>
+  </si>
+  <si>
+    <t>2 exons, necessary domains present</t>
+  </si>
+  <si>
+    <t>2 exons, the second of which is too short.There is clearly RNAseq hits in the downstream region. I tried to shift around the exon to get a longer ORF for exon 2, although given the RNAseq data I'm not convinced this is accurate. However, the new protein is longer, and matched via Blastp to Ce-gcy-5, 7, 17, 14, etc... tblastn of protein back to S. ratti genome got me ,matches to SRAE_2000494300 (as does SSTP_0000937900. Looking at the Sr and Ss genomes, the genes flanking this one and SSTP_0000937900 are a 7M GPCR on the 5' forward strand, and a protein with an alpha/beta hydrolase on the 3' reverse strand. those same genes are flanking SRAE_2000494300).</t>
   </si>
 </sst>
 </file>
@@ -865,7 +933,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -875,6 +943,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -892,7 +972,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -903,6 +983,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1221,10 +1310,10 @@
   <dimension ref="A1:Z30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="22.5" customWidth="1"/>
@@ -1643,7 +1732,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>
@@ -1667,7 +1756,7 @@
         <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="K6" t="s">
         <v>21</v>
@@ -1732,7 +1821,7 @@
         <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="F7" t="s">
         <v>31</v>
@@ -1866,7 +1955,7 @@
         <v>18</v>
       </c>
       <c r="W8" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="X8" t="s">
         <v>22</v>
@@ -2112,7 +2201,7 @@
         <v>33</v>
       </c>
       <c r="Y11" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
@@ -2725,7 +2814,7 @@
         <v>35</v>
       </c>
       <c r="H25" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="I25" t="s">
         <v>35</v>
@@ -2745,7 +2834,7 @@
         <v>33</v>
       </c>
       <c r="E26" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="F26" t="s">
         <v>25</v>
@@ -2795,11 +2884,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4AF0C57-95CB-A24A-8D1E-C9EDB24C1D1D}">
   <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="26.6640625" customWidth="1"/>
@@ -3306,7 +3395,7 @@
         <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="D7" t="s">
         <v>49</v>
@@ -4512,7 +4601,7 @@
         <v>72</v>
       </c>
       <c r="L22" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="M22" t="s">
         <v>69</v>
@@ -4568,7 +4657,7 @@
         <v>67</v>
       </c>
       <c r="I23" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="J23" t="s">
         <v>73</v>
@@ -4783,7 +4872,7 @@
         <v>73</v>
       </c>
       <c r="U27" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
@@ -4915,7 +5004,7 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.6640625" customWidth="1"/>
   </cols>
@@ -4928,7 +5017,7 @@
         <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -4950,7 +5039,7 @@
         <v>52</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -5122,7 +5211,7 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" customWidth="1"/>
@@ -5132,16 +5221,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5245,7 +5334,7 @@
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -5269,7 +5358,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
@@ -5284,7 +5373,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
@@ -5344,7 +5433,7 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
@@ -5364,17 +5453,17 @@
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
@@ -5404,7 +5493,7 @@
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
@@ -5429,13 +5518,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{427D24AC-C616-B842-8203-23EFB599A2A4}">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:BE64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="34.83203125" customWidth="1"/>
     <col min="4" max="4" width="31.6640625" customWidth="1"/>
@@ -5443,1083 +5532,1480 @@
     <col min="6" max="6" width="47.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>259</v>
+        <v>206</v>
       </c>
       <c r="B2" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="E2" s="2">
         <v>462</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B3" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="E3" s="2">
         <v>255</v>
       </c>
       <c r="F3" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>259</v>
+        <v>206</v>
       </c>
       <c r="B4" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="E4" s="2">
         <v>178</v>
       </c>
       <c r="F4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="B5" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="E5" s="2">
         <v>160</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="B6" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="E6" s="2">
         <v>715</v>
       </c>
       <c r="F6" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="B7" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="E7" s="2">
         <v>698</v>
       </c>
       <c r="F7" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="B8" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="E8" s="7">
         <v>581</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="B9" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="E9" s="7">
         <v>332</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="B10" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="E10" s="2">
         <v>231</v>
       </c>
       <c r="F10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="B11" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="E11" s="2">
         <v>1778</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="B12" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="E12" s="2">
         <v>686</v>
       </c>
       <c r="F12" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+    </row>
+    <row r="13" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="B13" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="E13" s="2">
         <v>678</v>
       </c>
-      <c r="F13" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F13" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+    </row>
+    <row r="14" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="B14" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="E14" s="2">
         <v>548</v>
       </c>
-      <c r="F14" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F14" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+    </row>
+    <row r="15" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="B15" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E15" s="2">
         <v>332</v>
       </c>
-      <c r="F15" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F15" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="B16" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="E16" s="2">
         <v>245</v>
       </c>
-      <c r="F16" t="s">
-        <v>221</v>
-      </c>
+      <c r="F16" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="D17" t="s">
-        <v>238</v>
+        <v>219</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>220</v>
       </c>
       <c r="E17" s="4">
         <v>1781</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="D18" t="s">
-        <v>239</v>
+        <v>218</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>221</v>
       </c>
       <c r="E18" s="4">
         <v>1092</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="B19" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>158</v>
+        <v>241</v>
+      </c>
+      <c r="D19" t="s">
+        <v>239</v>
       </c>
       <c r="E19" s="2">
-        <v>1503</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>232</v>
-      </c>
-      <c r="B20" t="s">
-        <v>229</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E20" s="2">
-        <v>945</v>
+        <v>1540</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="D20" t="s">
+        <v>245</v>
+      </c>
+      <c r="E20" s="11">
+        <v>1006</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
+      <c r="A21" s="5" t="s">
+        <v>215</v>
+      </c>
       <c r="B21" s="5" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="E21" s="4">
         <v>1065</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
+      <c r="A22" s="5" t="s">
+        <v>215</v>
+      </c>
       <c r="B22" s="5" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
       <c r="E22" s="4">
         <v>1054</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>215</v>
+      </c>
       <c r="B23" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="E23" s="2">
         <v>1522</v>
       </c>
+      <c r="F23" s="4" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>215</v>
+      </c>
       <c r="B24" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E24" s="2">
         <v>1518</v>
       </c>
+      <c r="F24" s="4" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>215</v>
+      </c>
       <c r="B25" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>77</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E25" s="2">
         <v>1128</v>
       </c>
+      <c r="F25" s="4" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>215</v>
+      </c>
       <c r="B26" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>134</v>
+        <v>201</v>
+      </c>
+      <c r="D26" t="s">
+        <v>237</v>
       </c>
       <c r="E26" s="2">
         <v>1120</v>
       </c>
       <c r="F26" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>230</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E27" s="2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E27" s="9">
         <v>1120</v>
       </c>
+      <c r="F27" s="12" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>215</v>
+      </c>
       <c r="B28" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D28" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="E28" s="2">
         <v>1113</v>
       </c>
       <c r="F28" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="B29" s="13" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>230</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E29" s="2">
-        <v>1102</v>
+      <c r="C29" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="E29" s="14">
+        <v>1129</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>216</v>
+      </c>
       <c r="B30" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="E30" s="2">
         <v>1100</v>
       </c>
+      <c r="F30" s="2" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>264</v>
+      </c>
       <c r="B31" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E31" s="2">
         <v>1099</v>
       </c>
+      <c r="F31" s="2" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>264</v>
+      </c>
       <c r="B32" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="E32" s="2">
         <v>1087</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F32" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>215</v>
+      </c>
       <c r="B33" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="E33" s="2">
         <v>1083</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F33" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>215</v>
+      </c>
       <c r="B34" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>78</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E34" s="2">
         <v>1080</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F34" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>215</v>
+      </c>
       <c r="B35" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="E35" s="2">
         <v>1077</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
-        <v>230</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E36" s="2">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F35" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="D36" t="s">
+        <v>244</v>
+      </c>
+      <c r="E36" s="11">
+        <v>1003</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>215</v>
+      </c>
       <c r="B37" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E37" s="2">
         <v>1064</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F37" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>215</v>
+      </c>
       <c r="B38" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E38" s="2">
         <v>1061</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>216</v>
+      </c>
       <c r="B39" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E39" s="2">
         <v>1060</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F39" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>215</v>
+      </c>
       <c r="B40" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E40" s="2">
         <v>1060</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>215</v>
+      </c>
       <c r="B41" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="E41" s="2">
         <v>1059</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F41" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>215</v>
+      </c>
       <c r="B42" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="E42" s="2">
         <v>1027</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F42" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>215</v>
+      </c>
       <c r="B43" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="E43" s="2">
         <v>1222</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F43" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>215</v>
+      </c>
       <c r="B44" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="E44" s="2">
         <v>1153</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>261</v>
-      </c>
-      <c r="B45" t="s">
-        <v>229</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D45" s="2" t="s">
+      <c r="F44" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E45" s="9">
+        <v>1134</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="E46" s="9">
+        <v>1129</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>215</v>
+      </c>
+      <c r="B47" t="s">
+        <v>213</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E45" s="2">
-        <v>1135</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>229</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E46" s="2">
-        <v>1134</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
-        <v>229</v>
-      </c>
-      <c r="C47" s="2" t="s">
+      <c r="E47" s="2">
+        <v>1117</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>215</v>
+      </c>
+      <c r="B48" t="s">
+        <v>213</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E48" s="2">
+        <v>1104</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="6"/>
+      <c r="L48" s="6"/>
+      <c r="M48" s="6"/>
+      <c r="N48" s="6"/>
+      <c r="O48" s="6"/>
+      <c r="P48" s="6"/>
+      <c r="Q48" s="6"/>
+      <c r="R48" s="6"/>
+      <c r="S48" s="6"/>
+    </row>
+    <row r="49" spans="1:57" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>215</v>
+      </c>
+      <c r="B49" t="s">
+        <v>213</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E49" s="2">
+        <v>1102</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="6"/>
+      <c r="K49" s="6"/>
+      <c r="L49" s="6"/>
+      <c r="M49" s="6"/>
+      <c r="N49" s="6"/>
+      <c r="O49" s="6"/>
+      <c r="P49" s="6"/>
+      <c r="Q49" s="6"/>
+      <c r="R49" s="6"/>
+      <c r="S49" s="6"/>
+    </row>
+    <row r="50" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>215</v>
+      </c>
+      <c r="B50" t="s">
+        <v>213</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E50" s="2">
+        <v>1088</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="6"/>
+      <c r="K50" s="6"/>
+      <c r="L50" s="6"/>
+      <c r="M50" s="6"/>
+      <c r="N50" s="6"/>
+      <c r="O50" s="6"/>
+      <c r="P50" s="6"/>
+      <c r="Q50" s="6"/>
+      <c r="R50" s="6"/>
+      <c r="S50" s="6"/>
+    </row>
+    <row r="51" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>215</v>
+      </c>
+      <c r="B51" t="s">
+        <v>213</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D51" t="s">
+        <v>238</v>
+      </c>
+      <c r="E51" s="2">
+        <v>1123</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="52" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E52" s="4">
+        <v>1079</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="53" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E53" s="4">
+        <v>1076</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="54" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>215</v>
+      </c>
+      <c r="B54" t="s">
+        <v>213</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E54" s="2">
+        <v>1070</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="55" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>215</v>
+      </c>
+      <c r="B55" t="s">
+        <v>213</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E47" s="2">
-        <v>1129</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
-        <v>229</v>
-      </c>
-      <c r="C48" s="2" t="s">
+      <c r="D55" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E55" s="2">
+        <v>1069</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="56" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>215</v>
+      </c>
+      <c r="B56" t="s">
+        <v>213</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E48" s="2">
-        <v>1117</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49"/>
-      <c r="B49" t="s">
-        <v>229</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E49" s="2">
-        <v>1104</v>
-      </c>
-      <c r="F49"/>
-    </row>
-    <row r="50" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50"/>
-      <c r="B50" t="s">
-        <v>229</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E50" s="2">
-        <v>1102</v>
-      </c>
-      <c r="F50"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
-        <v>229</v>
-      </c>
-      <c r="C51" s="2" t="s">
+      <c r="D56" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E56" s="2">
+        <v>1065</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="57" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>215</v>
+      </c>
+      <c r="B57" t="s">
+        <v>213</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E51" s="2">
-        <v>1088</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
-        <v>229</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D52" s="2" t="s">
+      <c r="D57" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E57" s="2">
+        <v>1062</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="58" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>215</v>
+      </c>
+      <c r="B58" t="s">
+        <v>213</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="E52" s="2">
-        <v>1085</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="E53" s="4">
-        <v>1079</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="E54" s="4">
-        <v>1076</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
-        <v>229</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E55" s="2">
-        <v>1070</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
-        <v>229</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E56" s="2">
-        <v>1069</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
-        <v>229</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E57" s="2">
-        <v>1065</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
-        <v>229</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="E58" s="2">
         <v>1062</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F58" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="59" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>215</v>
+      </c>
       <c r="B59" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="E59" s="2">
-        <v>1062</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1060</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="60" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>215</v>
+      </c>
       <c r="B60" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="E60" s="2">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="61" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>215</v>
+      </c>
       <c r="B61" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E61" s="2">
-        <v>1059</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1056</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="62" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>215</v>
+      </c>
       <c r="B62" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="E62" s="2">
-        <v>1056</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B63" t="s">
-        <v>229</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E63" s="2">
         <v>1055</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64"/>
-      <c r="B64" t="s">
-        <v>229</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E64" s="2">
-        <v>1033</v>
-      </c>
-      <c r="F64"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="E65" s="4">
-        <v>1033</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>253</v>
-      </c>
+      <c r="F62" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="63" spans="1:57" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D63" t="s">
+        <v>260</v>
+      </c>
+      <c r="E63" s="9">
+        <v>1118</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="15"/>
+      <c r="K63" s="15"/>
+      <c r="L63" s="15"/>
+      <c r="M63" s="15"/>
+      <c r="N63" s="15"/>
+      <c r="O63" s="15"/>
+      <c r="P63" s="15"/>
+      <c r="Q63" s="15"/>
+      <c r="R63" s="15"/>
+      <c r="S63" s="15"/>
+      <c r="T63" s="15"/>
+      <c r="U63" s="15"/>
+      <c r="V63" s="15"/>
+      <c r="W63" s="15"/>
+      <c r="X63" s="15"/>
+      <c r="Y63" s="15"/>
+      <c r="Z63" s="15"/>
+      <c r="AA63" s="15"/>
+      <c r="AB63" s="15"/>
+      <c r="AC63" s="15"/>
+      <c r="AD63" s="15"/>
+      <c r="AE63" s="15"/>
+      <c r="AF63" s="15"/>
+      <c r="AG63" s="15"/>
+      <c r="AH63" s="15"/>
+      <c r="AI63" s="15"/>
+      <c r="AJ63" s="15"/>
+      <c r="AK63" s="15"/>
+      <c r="AL63" s="15"/>
+      <c r="AM63" s="15"/>
+      <c r="AN63" s="15"/>
+      <c r="AO63" s="15"/>
+      <c r="AP63" s="15"/>
+      <c r="AQ63" s="15"/>
+      <c r="AR63" s="15"/>
+      <c r="AS63" s="15"/>
+      <c r="AT63" s="15"/>
+      <c r="AU63" s="15"/>
+      <c r="AV63" s="15"/>
+      <c r="AW63" s="15"/>
+      <c r="AX63" s="15"/>
+      <c r="AY63" s="15"/>
+      <c r="AZ63" s="15"/>
+      <c r="BA63" s="15"/>
+      <c r="BB63" s="15"/>
+      <c r="BC63" s="15"/>
+      <c r="BD63" s="15"/>
+      <c r="BE63" s="15"/>
+    </row>
+    <row r="64" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A64" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="D64" t="s">
+        <v>211</v>
+      </c>
+      <c r="E64" s="4">
+        <v>1032</v>
+      </c>
+      <c r="F64" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="6"/>
+      <c r="L64" s="6"/>
+      <c r="M64" s="6"/>
+      <c r="N64" s="6"/>
+      <c r="O64" s="6"/>
+      <c r="P64" s="6"/>
+      <c r="Q64" s="6"/>
+      <c r="R64" s="6"/>
+      <c r="S64" s="6"/>
+      <c r="T64" s="6"/>
+      <c r="U64" s="6"/>
+      <c r="V64" s="6"/>
+      <c r="W64" s="6"/>
+      <c r="X64" s="6"/>
+      <c r="Y64" s="6"/>
+      <c r="Z64" s="6"/>
+      <c r="AA64" s="6"/>
+      <c r="AB64" s="6"/>
+      <c r="AC64" s="6"/>
+      <c r="AD64" s="6"/>
+      <c r="AE64" s="6"/>
+      <c r="AF64" s="6"/>
+      <c r="AG64" s="6"/>
+      <c r="AH64" s="6"/>
+      <c r="AI64" s="6"/>
+      <c r="AJ64" s="6"/>
+      <c r="AK64" s="6"/>
+      <c r="AL64" s="6"/>
+      <c r="AM64" s="6"/>
+      <c r="AN64" s="6"/>
+      <c r="AO64" s="6"/>
+      <c r="AP64" s="6"/>
+      <c r="AQ64" s="6"/>
+      <c r="AR64" s="6"/>
+      <c r="AS64" s="6"/>
+      <c r="AT64" s="6"/>
+      <c r="AU64" s="6"/>
+      <c r="AV64" s="6"/>
+      <c r="AW64" s="6"/>
+      <c r="AX64" s="6"/>
+      <c r="AY64" s="6"/>
+      <c r="AZ64" s="6"/>
+      <c r="BA64" s="6"/>
+      <c r="BB64" s="6"/>
+      <c r="BC64" s="6"/>
+      <c r="BD64" s="6"/>
+      <c r="BE64" s="6"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
-    <sortCondition ref="A2:A65"/>
-    <sortCondition ref="B2:B65"/>
-    <sortCondition descending="1" ref="E2:E65"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F64">
+    <sortCondition ref="A2:A64"/>
+    <sortCondition ref="B2:B64"/>
+    <sortCondition descending="1" ref="E2:E64"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>